<commit_message>
AD process model Magazines_ to Magazine
</commit_message>
<xml_diff>
--- a/Material properties - process modles.xlsx
+++ b/Material properties - process modles.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msmsa\Google Drive\Brightway2\Material properties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msardar2\Google Drive\Brightway2\Laptop_BitBucket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5ABE0C-D3AE-4675-863C-F451D0846CFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Composting" sheetId="1" r:id="rId1"/>
@@ -540,9 +539,6 @@
     <t>Office_Paper</t>
   </si>
   <si>
-    <t>Magazines_</t>
-  </si>
-  <si>
     <t>third_Class_Mail</t>
   </si>
   <si>
@@ -685,12 +681,15 @@
   </si>
   <si>
     <t>Fraction of Cu that is Recoverable</t>
+  </si>
+  <si>
+    <t>Magazines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -973,7 +972,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1216,62 +1215,59 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="51">
-    <cellStyle name="Currency 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Currency 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Hyperlink 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="27" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Currency 2" xfId="40"/>
+    <cellStyle name="Currency 3" xfId="26"/>
+    <cellStyle name="Hyperlink 2" xfId="32"/>
+    <cellStyle name="Hyperlink 3" xfId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 2 2 3" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 2 2 4" xfId="14" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 2 2 5" xfId="17" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 2 2 6" xfId="20" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 2 2 7" xfId="23" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 2 2 8" xfId="8" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 2 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 2 3 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 2 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 2 4 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 2 5" xfId="16" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 2 5 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 2 6" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Normal 2 6 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 2 7" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 2 7 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 3 3" xfId="38" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 4" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 4 2" xfId="39" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 6" xfId="15" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 6 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 7" xfId="21" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 8" xfId="2" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 8 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 8 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 8 3" xfId="28" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 8 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 9" xfId="30" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 9 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Normal 9 3" xfId="48" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Normal_changes" xfId="3" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal_MRF" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 2 2" xfId="6"/>
+    <cellStyle name="Normal 2 2 2" xfId="9"/>
+    <cellStyle name="Normal 2 2 3" xfId="12"/>
+    <cellStyle name="Normal 2 2 4" xfId="14"/>
+    <cellStyle name="Normal 2 2 5" xfId="17"/>
+    <cellStyle name="Normal 2 2 6" xfId="20"/>
+    <cellStyle name="Normal 2 2 7" xfId="23"/>
+    <cellStyle name="Normal 2 2 8" xfId="8"/>
+    <cellStyle name="Normal 2 3" xfId="11"/>
+    <cellStyle name="Normal 2 3 2" xfId="33"/>
+    <cellStyle name="Normal 2 4" xfId="10"/>
+    <cellStyle name="Normal 2 4 2" xfId="34"/>
+    <cellStyle name="Normal 2 5" xfId="16"/>
+    <cellStyle name="Normal 2 5 2" xfId="35"/>
+    <cellStyle name="Normal 2 6" xfId="19"/>
+    <cellStyle name="Normal 2 6 2" xfId="36"/>
+    <cellStyle name="Normal 2 7" xfId="22"/>
+    <cellStyle name="Normal 2 7 2" xfId="37"/>
+    <cellStyle name="Normal 3" xfId="18"/>
+    <cellStyle name="Normal 3 2" xfId="31"/>
+    <cellStyle name="Normal 3 2 2" xfId="44"/>
+    <cellStyle name="Normal 3 3" xfId="38"/>
+    <cellStyle name="Normal 4" xfId="24"/>
+    <cellStyle name="Normal 4 2" xfId="39"/>
+    <cellStyle name="Normal 5" xfId="13"/>
+    <cellStyle name="Normal 6" xfId="15"/>
+    <cellStyle name="Normal 6 2" xfId="46"/>
+    <cellStyle name="Normal 7" xfId="21"/>
+    <cellStyle name="Normal 8" xfId="2"/>
+    <cellStyle name="Normal 8 2" xfId="41"/>
+    <cellStyle name="Normal 8 2 2" xfId="50"/>
+    <cellStyle name="Normal 8 3" xfId="28"/>
+    <cellStyle name="Normal 8 4" xfId="47"/>
+    <cellStyle name="Normal 9" xfId="30"/>
+    <cellStyle name="Normal 9 2" xfId="43"/>
+    <cellStyle name="Normal 9 3" xfId="48"/>
+    <cellStyle name="Normal_changes" xfId="3"/>
+    <cellStyle name="Normal_MRF" xfId="45"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Percent 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Percent 3" xfId="25" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Percent 3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Percent 3 3" xfId="29" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Percent 3 4" xfId="49" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Percent 2" xfId="4"/>
+    <cellStyle name="Percent 2 2" xfId="7"/>
+    <cellStyle name="Percent 3" xfId="25"/>
+    <cellStyle name="Percent 3 2" xfId="42"/>
+    <cellStyle name="Percent 3 3" xfId="29"/>
+    <cellStyle name="Percent 3 4" xfId="49"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1548,23 +1544,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="25.54296875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="25.5703125" style="19" customWidth="1"/>
     <col min="14" max="14" width="31" style="22" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="63" width="25.54296875" style="19" customWidth="1"/>
-    <col min="64" max="16384" width="9.1796875" style="19"/>
+    <col min="16" max="63" width="25.5703125" style="19" customWidth="1"/>
+    <col min="64" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="16" customFormat="1" ht="81" customHeight="1">
@@ -2174,7 +2170,7 @@
     <row r="17" spans="1:15">
       <c r="A17" s="8"/>
       <c r="B17" s="83" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="C17" s="9">
         <v>95</v>
@@ -2213,7 +2209,7 @@
     <row r="18" spans="1:15">
       <c r="A18" s="8"/>
       <c r="B18" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="9">
         <v>95</v>
@@ -2252,7 +2248,7 @@
     <row r="19" spans="1:15">
       <c r="A19" s="8"/>
       <c r="B19" s="83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="9">
         <v>95</v>
@@ -2291,7 +2287,7 @@
     <row r="20" spans="1:15">
       <c r="A20" s="8"/>
       <c r="B20" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="9">
         <v>95</v>
@@ -2330,7 +2326,7 @@
     <row r="21" spans="1:15">
       <c r="A21" s="8"/>
       <c r="B21" s="83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="9">
         <v>95</v>
@@ -2369,7 +2365,7 @@
     <row r="22" spans="1:15">
       <c r="A22" s="8"/>
       <c r="B22" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="9">
         <v>95</v>
@@ -2408,7 +2404,7 @@
     <row r="23" spans="1:15">
       <c r="A23" s="8"/>
       <c r="B23" s="83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="9">
         <v>95</v>
@@ -2447,7 +2443,7 @@
     <row r="24" spans="1:15">
       <c r="A24" s="8"/>
       <c r="B24" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="9">
         <v>95</v>
@@ -2486,7 +2482,7 @@
     <row r="25" spans="1:15">
       <c r="A25" s="8"/>
       <c r="B25" s="83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="9">
         <v>95</v>
@@ -2525,7 +2521,7 @@
     <row r="26" spans="1:15">
       <c r="A26" s="8"/>
       <c r="B26" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="9">
         <v>95</v>
@@ -2564,7 +2560,7 @@
     <row r="27" spans="1:15">
       <c r="A27" s="8"/>
       <c r="B27" s="83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="9">
         <v>95</v>
@@ -2603,7 +2599,7 @@
     <row r="28" spans="1:15">
       <c r="A28" s="8"/>
       <c r="B28" s="83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="9">
         <v>95</v>
@@ -2642,7 +2638,7 @@
     <row r="29" spans="1:15">
       <c r="A29" s="8"/>
       <c r="B29" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="9">
         <v>95</v>
@@ -2681,7 +2677,7 @@
     <row r="30" spans="1:15">
       <c r="A30" s="8"/>
       <c r="B30" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C30" s="9">
         <v>95</v>
@@ -2720,7 +2716,7 @@
     <row r="31" spans="1:15">
       <c r="A31" s="8"/>
       <c r="B31" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C31" s="9">
         <v>95</v>
@@ -2759,7 +2755,7 @@
     <row r="32" spans="1:15">
       <c r="A32" s="8"/>
       <c r="B32" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="9">
         <v>95</v>
@@ -2798,7 +2794,7 @@
     <row r="33" spans="1:15">
       <c r="A33" s="8"/>
       <c r="B33" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="9">
         <v>95</v>
@@ -2837,7 +2833,7 @@
     <row r="34" spans="1:15">
       <c r="A34" s="8"/>
       <c r="B34" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C34" s="9">
         <v>95</v>
@@ -2876,7 +2872,7 @@
     <row r="35" spans="1:15">
       <c r="A35" s="8"/>
       <c r="B35" s="83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="9">
         <v>95</v>
@@ -2915,7 +2911,7 @@
     <row r="36" spans="1:15">
       <c r="A36" s="8"/>
       <c r="B36" s="83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C36" s="9">
         <v>95</v>
@@ -2954,7 +2950,7 @@
     <row r="37" spans="1:15">
       <c r="A37" s="8"/>
       <c r="B37" s="83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="9">
         <v>95</v>
@@ -2993,7 +2989,7 @@
     <row r="38" spans="1:15">
       <c r="A38" s="8"/>
       <c r="B38" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="9">
         <v>95</v>
@@ -3032,7 +3028,7 @@
     <row r="39" spans="1:15">
       <c r="A39" s="8"/>
       <c r="B39" s="83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C39" s="9">
         <v>95</v>
@@ -3071,7 +3067,7 @@
     <row r="40" spans="1:15">
       <c r="A40" s="8"/>
       <c r="B40" s="83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C40" s="9">
         <v>95</v>
@@ -3110,7 +3106,7 @@
     <row r="41" spans="1:15">
       <c r="A41" s="8"/>
       <c r="B41" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C41" s="9">
         <v>95</v>
@@ -3149,7 +3145,7 @@
     <row r="42" spans="1:15">
       <c r="A42" s="8"/>
       <c r="B42" s="83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="9">
         <v>95</v>
@@ -3188,7 +3184,7 @@
     <row r="43" spans="1:15">
       <c r="A43" s="8"/>
       <c r="B43" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="9">
         <v>95</v>
@@ -3227,7 +3223,7 @@
     <row r="44" spans="1:15">
       <c r="A44" s="8"/>
       <c r="B44" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44" s="9">
         <v>5</v>
@@ -3266,7 +3262,7 @@
     <row r="45" spans="1:15">
       <c r="A45" s="8"/>
       <c r="B45" s="83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="9">
         <v>95</v>
@@ -3305,7 +3301,7 @@
     <row r="46" spans="1:15">
       <c r="A46" s="8"/>
       <c r="B46" s="83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="9">
         <v>0</v>
@@ -3344,7 +3340,7 @@
     <row r="47" spans="1:15">
       <c r="A47" s="8"/>
       <c r="B47" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" s="9">
         <v>0</v>
@@ -3383,7 +3379,7 @@
     <row r="48" spans="1:15">
       <c r="A48" s="8"/>
       <c r="B48" s="83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -3422,7 +3418,7 @@
     <row r="49" spans="1:15">
       <c r="A49" s="8"/>
       <c r="B49" s="83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C49" s="9">
         <v>0</v>
@@ -3461,7 +3457,7 @@
     <row r="50" spans="1:15">
       <c r="A50" s="8"/>
       <c r="B50" s="83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="9">
         <v>0</v>
@@ -3500,7 +3496,7 @@
     <row r="51" spans="1:15">
       <c r="A51" s="8"/>
       <c r="B51" s="83" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" s="9">
         <v>0</v>
@@ -3539,7 +3535,7 @@
     <row r="52" spans="1:15">
       <c r="A52" s="8"/>
       <c r="B52" s="83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C52" s="9">
         <v>0</v>
@@ -3578,7 +3574,7 @@
     <row r="53" spans="1:15">
       <c r="A53" s="8"/>
       <c r="B53" s="83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C53" s="9">
         <v>0</v>
@@ -3617,7 +3613,7 @@
     <row r="54" spans="1:15">
       <c r="A54" s="8"/>
       <c r="B54" s="83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C54" s="9">
         <v>0</v>
@@ -3656,7 +3652,7 @@
     <row r="55" spans="1:15">
       <c r="A55" s="8"/>
       <c r="B55" s="83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C55" s="9">
         <v>0</v>
@@ -3695,7 +3691,7 @@
     <row r="56" spans="1:15">
       <c r="A56" s="8"/>
       <c r="B56" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C56" s="9">
         <v>0</v>
@@ -3734,7 +3730,7 @@
     <row r="57" spans="1:15">
       <c r="A57" s="8"/>
       <c r="B57" s="83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C57" s="9">
         <v>0</v>
@@ -3773,7 +3769,7 @@
     <row r="58" spans="1:15">
       <c r="A58" s="8"/>
       <c r="B58" s="83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C58" s="9">
         <v>0</v>
@@ -3812,7 +3808,7 @@
     <row r="59" spans="1:15">
       <c r="A59" s="8"/>
       <c r="B59" s="83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="9">
         <v>0</v>
@@ -3851,7 +3847,7 @@
     <row r="60" spans="1:15">
       <c r="A60" s="8"/>
       <c r="B60" s="83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C60" s="9">
         <v>0</v>
@@ -3890,7 +3886,7 @@
     <row r="61" spans="1:15">
       <c r="A61" s="8"/>
       <c r="B61" s="83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="9">
         <v>0</v>
@@ -3929,7 +3925,7 @@
     <row r="62" spans="1:15">
       <c r="A62" s="8"/>
       <c r="B62" s="83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="9">
         <v>0</v>
@@ -3968,7 +3964,7 @@
     <row r="63" spans="1:15">
       <c r="A63" s="8"/>
       <c r="B63" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C63" s="9">
         <v>0</v>
@@ -4007,7 +4003,7 @@
     <row r="64" spans="1:15">
       <c r="A64" s="8"/>
       <c r="B64" s="83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C64" s="9">
         <v>0</v>
@@ -4049,18 +4045,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="20.81640625" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="19"/>
+    <col min="2" max="9" width="20.85546875" style="19" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="33" customFormat="1" ht="81" customHeight="1">
@@ -4156,7 +4152,7 @@
       <c r="I4" s="29"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="83" t="s">
         <v>160</v>
       </c>
       <c r="B5" s="25"/>
@@ -4183,7 +4179,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="83" t="s">
         <v>161</v>
       </c>
       <c r="B6" s="25"/>
@@ -4210,7 +4206,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="83" t="s">
         <v>162</v>
       </c>
       <c r="B7" s="25"/>
@@ -4237,7 +4233,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="83" t="s">
         <v>163</v>
       </c>
       <c r="B8" s="25"/>
@@ -4264,7 +4260,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="83" t="s">
         <v>164</v>
       </c>
       <c r="B9" s="25"/>
@@ -4291,7 +4287,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="83" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="25"/>
@@ -4318,7 +4314,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="86" t="s">
+      <c r="A11" s="83" t="s">
         <v>165</v>
       </c>
       <c r="B11" s="25"/>
@@ -4345,7 +4341,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="86" t="s">
+      <c r="A12" s="83" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="25"/>
@@ -4372,7 +4368,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="86" t="s">
+      <c r="A13" s="83" t="s">
         <v>166</v>
       </c>
       <c r="B13" s="25"/>
@@ -4399,7 +4395,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="83" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="25"/>
@@ -4426,7 +4422,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="83" t="s">
         <v>167</v>
       </c>
       <c r="B15" s="25"/>
@@ -4453,7 +4449,7 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="83" t="s">
         <v>168</v>
       </c>
       <c r="B16" s="25"/>
@@ -4480,8 +4476,8 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="86" t="s">
-        <v>169</v>
+      <c r="A17" s="83" t="s">
+        <v>217</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="25">
@@ -4507,8 +4503,8 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="86" t="s">
-        <v>170</v>
+      <c r="A18" s="83" t="s">
+        <v>169</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25">
@@ -4534,8 +4530,8 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="86" t="s">
-        <v>171</v>
+      <c r="A19" s="83" t="s">
+        <v>170</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="25">
@@ -4561,8 +4557,8 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="86" t="s">
-        <v>172</v>
+      <c r="A20" s="83" t="s">
+        <v>171</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="25">
@@ -4588,8 +4584,8 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="86" t="s">
-        <v>173</v>
+      <c r="A21" s="83" t="s">
+        <v>172</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="25">
@@ -4615,8 +4611,8 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="86" t="s">
-        <v>174</v>
+      <c r="A22" s="83" t="s">
+        <v>173</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="25">
@@ -4642,8 +4638,8 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="86" t="s">
-        <v>175</v>
+      <c r="A23" s="83" t="s">
+        <v>174</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="25">
@@ -4669,8 +4665,8 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="86" t="s">
-        <v>176</v>
+      <c r="A24" s="83" t="s">
+        <v>175</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="25">
@@ -4696,8 +4692,8 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="86" t="s">
-        <v>177</v>
+      <c r="A25" s="83" t="s">
+        <v>176</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="25">
@@ -4723,8 +4719,8 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="86" t="s">
-        <v>178</v>
+      <c r="A26" s="83" t="s">
+        <v>177</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="25">
@@ -4750,8 +4746,8 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="86" t="s">
-        <v>179</v>
+      <c r="A27" s="83" t="s">
+        <v>178</v>
       </c>
       <c r="B27" s="25"/>
       <c r="C27" s="25">
@@ -4777,8 +4773,8 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="86" t="s">
-        <v>180</v>
+      <c r="A28" s="83" t="s">
+        <v>179</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="25">
@@ -4804,8 +4800,8 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="86" t="s">
-        <v>181</v>
+      <c r="A29" s="83" t="s">
+        <v>180</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="25">
@@ -4831,8 +4827,8 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="86" t="s">
-        <v>182</v>
+      <c r="A30" s="83" t="s">
+        <v>181</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="25">
@@ -4858,8 +4854,8 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="86" t="s">
-        <v>183</v>
+      <c r="A31" s="83" t="s">
+        <v>182</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="25">
@@ -4885,8 +4881,8 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="86" t="s">
-        <v>184</v>
+      <c r="A32" s="83" t="s">
+        <v>183</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="25">
@@ -4912,8 +4908,8 @@
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="86" t="s">
-        <v>185</v>
+      <c r="A33" s="83" t="s">
+        <v>184</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="25">
@@ -4939,8 +4935,8 @@
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="86" t="s">
-        <v>186</v>
+      <c r="A34" s="83" t="s">
+        <v>185</v>
       </c>
       <c r="B34" s="25"/>
       <c r="C34" s="25">
@@ -4966,8 +4962,8 @@
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="86" t="s">
-        <v>187</v>
+      <c r="A35" s="83" t="s">
+        <v>186</v>
       </c>
       <c r="B35" s="25"/>
       <c r="C35" s="25">
@@ -4993,8 +4989,8 @@
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="86" t="s">
-        <v>188</v>
+      <c r="A36" s="83" t="s">
+        <v>187</v>
       </c>
       <c r="B36" s="25"/>
       <c r="C36" s="25">
@@ -5020,8 +5016,8 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="86" t="s">
-        <v>189</v>
+      <c r="A37" s="83" t="s">
+        <v>188</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="25">
@@ -5047,8 +5043,8 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="86" t="s">
-        <v>190</v>
+      <c r="A38" s="83" t="s">
+        <v>189</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25">
@@ -5074,8 +5070,8 @@
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="86" t="s">
-        <v>191</v>
+      <c r="A39" s="83" t="s">
+        <v>190</v>
       </c>
       <c r="B39" s="25"/>
       <c r="C39" s="25">
@@ -5101,8 +5097,8 @@
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="86" t="s">
-        <v>192</v>
+      <c r="A40" s="83" t="s">
+        <v>191</v>
       </c>
       <c r="B40" s="25"/>
       <c r="C40" s="25">
@@ -5128,8 +5124,8 @@
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="86" t="s">
-        <v>193</v>
+      <c r="A41" s="83" t="s">
+        <v>192</v>
       </c>
       <c r="B41" s="25"/>
       <c r="C41" s="25">
@@ -5155,8 +5151,8 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="86" t="s">
-        <v>194</v>
+      <c r="A42" s="83" t="s">
+        <v>193</v>
       </c>
       <c r="B42" s="25"/>
       <c r="C42" s="25">
@@ -5182,8 +5178,8 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="86" t="s">
-        <v>195</v>
+      <c r="A43" s="83" t="s">
+        <v>194</v>
       </c>
       <c r="B43" s="25"/>
       <c r="C43" s="25">
@@ -5209,8 +5205,8 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="86" t="s">
-        <v>196</v>
+      <c r="A44" s="83" t="s">
+        <v>195</v>
       </c>
       <c r="B44" s="25"/>
       <c r="C44" s="25">
@@ -5236,8 +5232,8 @@
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="86" t="s">
-        <v>197</v>
+      <c r="A45" s="83" t="s">
+        <v>196</v>
       </c>
       <c r="B45" s="25"/>
       <c r="C45" s="25">
@@ -5263,8 +5259,8 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="86" t="s">
-        <v>198</v>
+      <c r="A46" s="83" t="s">
+        <v>197</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25">
@@ -5290,8 +5286,8 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="86" t="s">
-        <v>199</v>
+      <c r="A47" s="83" t="s">
+        <v>198</v>
       </c>
       <c r="B47" s="25"/>
       <c r="C47" s="25">
@@ -5317,8 +5313,8 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="86" t="s">
-        <v>200</v>
+      <c r="A48" s="83" t="s">
+        <v>199</v>
       </c>
       <c r="B48" s="25"/>
       <c r="C48" s="25">
@@ -5344,8 +5340,8 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="86" t="s">
-        <v>201</v>
+      <c r="A49" s="83" t="s">
+        <v>200</v>
       </c>
       <c r="B49" s="25"/>
       <c r="C49" s="25">
@@ -5371,8 +5367,8 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="86" t="s">
-        <v>202</v>
+      <c r="A50" s="83" t="s">
+        <v>201</v>
       </c>
       <c r="B50" s="25"/>
       <c r="C50" s="25"/>
@@ -5388,8 +5384,8 @@
       <c r="I50" s="25"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="86" t="s">
-        <v>203</v>
+      <c r="A51" s="83" t="s">
+        <v>202</v>
       </c>
       <c r="B51" s="25"/>
       <c r="C51" s="25"/>
@@ -5405,8 +5401,8 @@
       <c r="I51" s="25"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="86" t="s">
-        <v>204</v>
+      <c r="A52" s="83" t="s">
+        <v>203</v>
       </c>
       <c r="B52" s="25"/>
       <c r="C52" s="25"/>
@@ -5422,8 +5418,8 @@
       <c r="I52" s="25"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="86" t="s">
-        <v>205</v>
+      <c r="A53" s="83" t="s">
+        <v>204</v>
       </c>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
@@ -5439,8 +5435,8 @@
       <c r="I53" s="25"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="86" t="s">
-        <v>206</v>
+      <c r="A54" s="83" t="s">
+        <v>205</v>
       </c>
       <c r="B54" s="25"/>
       <c r="C54" s="25"/>
@@ -5456,8 +5452,8 @@
       <c r="I54" s="25"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="86" t="s">
-        <v>207</v>
+      <c r="A55" s="83" t="s">
+        <v>206</v>
       </c>
       <c r="B55" s="25"/>
       <c r="C55" s="25"/>
@@ -5473,8 +5469,8 @@
       <c r="I55" s="25"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="86" t="s">
-        <v>208</v>
+      <c r="A56" s="83" t="s">
+        <v>207</v>
       </c>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
@@ -5490,8 +5486,8 @@
       <c r="I56" s="25"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="86" t="s">
-        <v>209</v>
+      <c r="A57" s="83" t="s">
+        <v>208</v>
       </c>
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
@@ -5507,8 +5503,8 @@
       <c r="I57" s="25"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="86" t="s">
-        <v>210</v>
+      <c r="A58" s="83" t="s">
+        <v>209</v>
       </c>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -5524,8 +5520,8 @@
       <c r="I58" s="25"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="86" t="s">
-        <v>211</v>
+      <c r="A59" s="83" t="s">
+        <v>210</v>
       </c>
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
@@ -5541,8 +5537,8 @@
       <c r="I59" s="25"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="86" t="s">
-        <v>212</v>
+      <c r="A60" s="83" t="s">
+        <v>211</v>
       </c>
       <c r="B60" s="25"/>
       <c r="C60" s="25"/>
@@ -5558,8 +5554,8 @@
       <c r="I60" s="25"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="86" t="s">
-        <v>213</v>
+      <c r="A61" s="83" t="s">
+        <v>212</v>
       </c>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
@@ -5575,8 +5571,8 @@
       <c r="I61" s="25"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="86" t="s">
-        <v>214</v>
+      <c r="A62" s="83" t="s">
+        <v>213</v>
       </c>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
@@ -5592,8 +5588,8 @@
       <c r="I62" s="25"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="86" t="s">
-        <v>215</v>
+      <c r="A63" s="83" t="s">
+        <v>214</v>
       </c>
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
@@ -5609,8 +5605,8 @@
       <c r="I63" s="25"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="86" t="s">
-        <v>216</v>
+      <c r="A64" s="83" t="s">
+        <v>215</v>
       </c>
       <c r="B64" s="25"/>
       <c r="C64" s="25"/>
@@ -5649,30 +5645,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.7265625" style="58" customWidth="1"/>
-    <col min="2" max="2" width="52.453125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" style="58" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="35"/>
+    <col min="11" max="11" width="28.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="44" customFormat="1" ht="58">
+    <row r="1" spans="1:16" s="44" customFormat="1" ht="60">
       <c r="A1" s="41" t="s">
         <v>94</v>
       </c>
@@ -5978,7 +5974,7 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="83" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -5992,7 +5988,7 @@
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
@@ -6006,7 +6002,7 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -6020,7 +6016,7 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
@@ -6034,7 +6030,7 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="39"/>
       <c r="D21" s="39"/>
@@ -6048,7 +6044,7 @@
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
@@ -6062,7 +6058,7 @@
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
@@ -6076,7 +6072,7 @@
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
@@ -6095,7 +6091,7 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -6114,7 +6110,7 @@
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -6133,7 +6129,7 @@
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
@@ -6152,7 +6148,7 @@
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
@@ -6171,7 +6167,7 @@
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
@@ -6190,7 +6186,7 @@
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
@@ -6209,7 +6205,7 @@
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
@@ -6238,7 +6234,7 @@
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
@@ -6267,7 +6263,7 @@
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
@@ -6294,7 +6290,7 @@
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
@@ -6321,7 +6317,7 @@
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>
@@ -6348,7 +6344,7 @@
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
@@ -6377,7 +6373,7 @@
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="39"/>
       <c r="D37" s="39"/>
@@ -6404,7 +6400,7 @@
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
@@ -6427,7 +6423,7 @@
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C39" s="39"/>
       <c r="D39" s="39"/>
@@ -6450,7 +6446,7 @@
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>
@@ -6473,7 +6469,7 @@
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C41" s="39"/>
       <c r="D41" s="39"/>
@@ -6496,7 +6492,7 @@
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="38"/>
       <c r="D42" s="38"/>
@@ -6519,7 +6515,7 @@
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="39"/>
       <c r="D43" s="39"/>
@@ -6538,7 +6534,7 @@
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44" s="38"/>
       <c r="D44" s="38"/>
@@ -6561,7 +6557,7 @@
     </row>
     <row r="45" spans="2:19">
       <c r="B45" s="83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="39"/>
       <c r="D45" s="39"/>
@@ -6584,7 +6580,7 @@
     </row>
     <row r="46" spans="2:19">
       <c r="B46" s="83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="38"/>
       <c r="D46" s="38"/>
@@ -6607,7 +6603,7 @@
     </row>
     <row r="47" spans="2:19">
       <c r="B47" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" s="39"/>
       <c r="D47" s="39"/>
@@ -6630,7 +6626,7 @@
     </row>
     <row r="48" spans="2:19">
       <c r="B48" s="83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48" s="38"/>
       <c r="D48" s="38"/>
@@ -6653,7 +6649,7 @@
     </row>
     <row r="49" spans="2:19">
       <c r="B49" s="83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C49" s="39"/>
       <c r="D49" s="39"/>
@@ -6676,7 +6672,7 @@
     </row>
     <row r="50" spans="2:19">
       <c r="B50" s="83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="38"/>
       <c r="D50" s="38"/>
@@ -6699,7 +6695,7 @@
     </row>
     <row r="51" spans="2:19">
       <c r="B51" s="83" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" s="39"/>
       <c r="D51" s="39"/>
@@ -6718,7 +6714,7 @@
     </row>
     <row r="52" spans="2:19">
       <c r="B52" s="83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C52" s="38"/>
       <c r="D52" s="38"/>
@@ -6737,7 +6733,7 @@
     </row>
     <row r="53" spans="2:19">
       <c r="B53" s="83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C53" s="39"/>
       <c r="D53" s="39"/>
@@ -6756,7 +6752,7 @@
     </row>
     <row r="54" spans="2:19">
       <c r="B54" s="83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C54" s="38"/>
       <c r="D54" s="38"/>
@@ -6775,7 +6771,7 @@
     </row>
     <row r="55" spans="2:19">
       <c r="B55" s="83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C55" s="39"/>
       <c r="D55" s="39"/>
@@ -6794,7 +6790,7 @@
     </row>
     <row r="56" spans="2:19">
       <c r="B56" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C56" s="38"/>
       <c r="D56" s="38"/>
@@ -6813,7 +6809,7 @@
     </row>
     <row r="57" spans="2:19">
       <c r="B57" s="83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C57" s="39"/>
       <c r="D57" s="39"/>
@@ -6832,7 +6828,7 @@
     </row>
     <row r="58" spans="2:19">
       <c r="B58" s="83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C58" s="38"/>
       <c r="D58" s="38"/>
@@ -6851,7 +6847,7 @@
     </row>
     <row r="59" spans="2:19">
       <c r="B59" s="83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="39"/>
       <c r="D59" s="39"/>
@@ -6870,7 +6866,7 @@
     </row>
     <row r="60" spans="2:19">
       <c r="B60" s="83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C60" s="38"/>
       <c r="D60" s="38"/>
@@ -6889,7 +6885,7 @@
     </row>
     <row r="61" spans="2:19">
       <c r="B61" s="83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="39"/>
       <c r="D61" s="39"/>
@@ -6908,7 +6904,7 @@
     </row>
     <row r="62" spans="2:19">
       <c r="B62" s="83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="38"/>
       <c r="D62" s="38"/>
@@ -6927,7 +6923,7 @@
     </row>
     <row r="63" spans="2:19">
       <c r="B63" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C63" s="39"/>
       <c r="D63" s="39"/>
@@ -6946,7 +6942,7 @@
     </row>
     <row r="64" spans="2:19">
       <c r="B64" s="83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C64" s="38"/>
       <c r="D64" s="38"/>
@@ -6969,30 +6965,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.453125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="58" customWidth="1"/>
     <col min="2" max="2" width="42" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7265625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1796875" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.54296875" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.7265625" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" style="58" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37" style="58" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44" style="58" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="37" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.54296875" style="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.5703125" style="58" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="58"/>
+    <col min="12" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="16" customFormat="1" ht="29">
+    <row r="1" spans="1:12" s="16" customFormat="1" ht="30">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
@@ -7021,7 +7017,7 @@
         <v>111</v>
       </c>
       <c r="J1" s="54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K1" s="54" t="s">
         <v>112</v>
@@ -7516,7 +7512,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="83" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="B17" s="39">
         <v>1</v>
@@ -7551,7 +7547,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B18" s="39">
         <v>1</v>
@@ -7586,7 +7582,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" s="39">
         <v>1</v>
@@ -7621,7 +7617,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B20" s="39">
         <v>1</v>
@@ -7656,7 +7652,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B21" s="39">
         <v>1</v>
@@ -7691,7 +7687,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B22" s="39">
         <v>1</v>
@@ -7726,7 +7722,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B23" s="39">
         <v>1</v>
@@ -7761,7 +7757,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B24" s="39">
         <v>1</v>
@@ -7796,7 +7792,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B25" s="39">
         <v>1</v>
@@ -7831,7 +7827,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" s="39">
         <v>1</v>
@@ -7866,7 +7862,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B27" s="39">
         <v>1</v>
@@ -7901,7 +7897,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B28" s="39">
         <v>1</v>
@@ -7936,7 +7932,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B29" s="39">
         <v>1</v>
@@ -7971,7 +7967,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30" s="39">
         <v>1</v>
@@ -8006,7 +8002,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B31" s="39">
         <v>1</v>
@@ -8041,7 +8037,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B32" s="39">
         <v>1</v>
@@ -8076,7 +8072,7 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B33" s="39">
         <v>1</v>
@@ -8111,7 +8107,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B34" s="39">
         <v>1</v>
@@ -8146,7 +8142,7 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B35" s="39">
         <v>1</v>
@@ -8181,7 +8177,7 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B36" s="39">
         <v>1</v>
@@ -8216,7 +8212,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B37" s="39">
         <v>1</v>
@@ -8251,7 +8247,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B38" s="39">
         <v>1</v>
@@ -8286,7 +8282,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B39" s="39">
         <v>1</v>
@@ -8321,7 +8317,7 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B40" s="39">
         <v>1</v>
@@ -8356,7 +8352,7 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B41" s="39">
         <v>1</v>
@@ -8391,7 +8387,7 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B42" s="39">
         <v>1</v>
@@ -8426,7 +8422,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B43" s="39">
         <v>1</v>
@@ -8461,7 +8457,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B44" s="39">
         <v>1</v>
@@ -8496,7 +8492,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B45" s="39">
         <v>1</v>
@@ -8531,7 +8527,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B46" s="39">
         <v>1</v>
@@ -8566,7 +8562,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B47" s="39">
         <v>1</v>
@@ -8601,7 +8597,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B48" s="39">
         <v>1</v>
@@ -8636,7 +8632,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B49" s="39">
         <v>1</v>
@@ -8671,7 +8667,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B50" s="39">
         <v>1</v>
@@ -8704,7 +8700,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="83" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B51" s="39">
         <v>1</v>
@@ -8737,7 +8733,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B52" s="39">
         <v>1</v>
@@ -8770,7 +8766,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B53" s="39">
         <v>1</v>
@@ -8803,7 +8799,7 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B54" s="39">
         <v>1</v>
@@ -8836,7 +8832,7 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B55" s="39">
         <v>1</v>
@@ -8869,7 +8865,7 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B56" s="39">
         <v>1</v>
@@ -8902,7 +8898,7 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B57" s="39">
         <v>1</v>
@@ -8935,7 +8931,7 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B58" s="39">
         <v>1</v>
@@ -8968,7 +8964,7 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B59" s="39">
         <v>1</v>
@@ -9001,7 +8997,7 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B60" s="39">
         <v>1</v>
@@ -9034,7 +9030,7 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B61" s="39">
         <v>1</v>
@@ -9067,7 +9063,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B62" s="39">
         <v>1</v>
@@ -9100,7 +9096,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B63" s="39">
         <v>1</v>
@@ -9133,7 +9129,7 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B64" s="39">
         <v>1</v>
@@ -9170,21 +9166,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.54296875" style="76" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" customWidth="1"/>
+    <col min="1" max="1" width="59.5703125" style="76" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
     <col min="3" max="30" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="66" customFormat="1" ht="58">
+    <row r="1" spans="1:30" s="66" customFormat="1" ht="60">
       <c r="A1" s="52" t="s">
         <v>94</v>
       </c>
@@ -9804,7 +9800,7 @@
     </row>
     <row r="17" spans="2:30">
       <c r="B17" s="83" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="C17" s="64"/>
       <c r="D17" s="64"/>
@@ -9845,7 +9841,7 @@
     </row>
     <row r="18" spans="2:30">
       <c r="B18" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="63"/>
       <c r="D18" s="63"/>
@@ -9886,7 +9882,7 @@
     </row>
     <row r="19" spans="2:30">
       <c r="B19" s="83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="64"/>
       <c r="D19" s="64"/>
@@ -9927,7 +9923,7 @@
     </row>
     <row r="20" spans="2:30">
       <c r="B20" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="63"/>
       <c r="D20" s="63"/>
@@ -9968,7 +9964,7 @@
     </row>
     <row r="21" spans="2:30">
       <c r="B21" s="83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="64"/>
       <c r="D21" s="64"/>
@@ -10009,7 +10005,7 @@
     </row>
     <row r="22" spans="2:30">
       <c r="B22" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
@@ -10042,7 +10038,7 @@
     </row>
     <row r="23" spans="2:30">
       <c r="B23" s="83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="64"/>
       <c r="D23" s="64"/>
@@ -10079,7 +10075,7 @@
     </row>
     <row r="24" spans="2:30">
       <c r="B24" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="63"/>
       <c r="D24" s="63"/>
@@ -10116,7 +10112,7 @@
     </row>
     <row r="25" spans="2:30">
       <c r="B25" s="83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="64"/>
       <c r="D25" s="64"/>
@@ -10153,7 +10149,7 @@
     </row>
     <row r="26" spans="2:30">
       <c r="B26" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="63"/>
       <c r="D26" s="63"/>
@@ -10186,7 +10182,7 @@
     </row>
     <row r="27" spans="2:30">
       <c r="B27" s="83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="64"/>
       <c r="D27" s="64"/>
@@ -10219,7 +10215,7 @@
     </row>
     <row r="28" spans="2:30">
       <c r="B28" s="83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="63"/>
       <c r="D28" s="63"/>
@@ -10252,7 +10248,7 @@
     </row>
     <row r="29" spans="2:30">
       <c r="B29" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="64"/>
       <c r="D29" s="64"/>
@@ -10291,7 +10287,7 @@
     </row>
     <row r="30" spans="2:30">
       <c r="B30" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C30" s="63"/>
       <c r="D30" s="63"/>
@@ -10324,7 +10320,7 @@
     </row>
     <row r="31" spans="2:30">
       <c r="B31" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C31" s="64"/>
       <c r="D31" s="64"/>
@@ -10361,7 +10357,7 @@
     </row>
     <row r="32" spans="2:30">
       <c r="B32" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="63"/>
       <c r="D32" s="63"/>
@@ -10398,7 +10394,7 @@
     </row>
     <row r="33" spans="2:30">
       <c r="B33" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="64">
         <v>0.88</v>
@@ -10435,7 +10431,7 @@
     </row>
     <row r="34" spans="2:30">
       <c r="B34" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C34" s="63">
         <v>0.88</v>
@@ -10472,7 +10468,7 @@
     </row>
     <row r="35" spans="2:30">
       <c r="B35" s="83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="64">
         <v>0.88</v>
@@ -10509,7 +10505,7 @@
     </row>
     <row r="36" spans="2:30">
       <c r="B36" s="83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C36" s="63"/>
       <c r="D36" s="63"/>
@@ -10546,7 +10542,7 @@
     </row>
     <row r="37" spans="2:30">
       <c r="B37" s="83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="64">
         <v>0.88</v>
@@ -10583,7 +10579,7 @@
     </row>
     <row r="38" spans="2:30">
       <c r="B38" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="63"/>
       <c r="D38" s="63"/>
@@ -10620,7 +10616,7 @@
     </row>
     <row r="39" spans="2:30">
       <c r="B39" s="83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C39" s="64"/>
       <c r="D39" s="64"/>
@@ -10657,7 +10653,7 @@
     </row>
     <row r="40" spans="2:30">
       <c r="B40" s="83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C40" s="63"/>
       <c r="D40" s="63"/>
@@ -10694,7 +10690,7 @@
     </row>
     <row r="41" spans="2:30">
       <c r="B41" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C41" s="64"/>
       <c r="D41" s="64"/>
@@ -10729,7 +10725,7 @@
     </row>
     <row r="42" spans="2:30">
       <c r="B42" s="83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="63"/>
       <c r="D42" s="63"/>
@@ -10764,7 +10760,7 @@
     </row>
     <row r="43" spans="2:30">
       <c r="B43" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="64"/>
       <c r="D43" s="64"/>
@@ -10797,7 +10793,7 @@
     </row>
     <row r="44" spans="2:30">
       <c r="B44" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44" s="63"/>
       <c r="D44" s="63"/>
@@ -10830,7 +10826,7 @@
     </row>
     <row r="45" spans="2:30">
       <c r="B45" s="83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="64"/>
@@ -10863,7 +10859,7 @@
     </row>
     <row r="46" spans="2:30">
       <c r="B46" s="83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="63"/>
       <c r="D46" s="63"/>
@@ -10896,7 +10892,7 @@
     </row>
     <row r="47" spans="2:30">
       <c r="B47" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" s="64"/>
       <c r="D47" s="64"/>
@@ -10929,7 +10925,7 @@
     </row>
     <row r="48" spans="2:30">
       <c r="B48" s="83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48" s="63"/>
       <c r="D48" s="63"/>
@@ -10962,7 +10958,7 @@
     </row>
     <row r="49" spans="2:30">
       <c r="B49" s="83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C49" s="64"/>
       <c r="D49" s="64"/>
@@ -10995,7 +10991,7 @@
     </row>
     <row r="50" spans="2:30">
       <c r="B50" s="83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="63"/>
       <c r="D50" s="63"/>
@@ -11028,7 +11024,7 @@
     </row>
     <row r="51" spans="2:30">
       <c r="B51" s="83" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" s="64"/>
       <c r="D51" s="64"/>
@@ -11061,7 +11057,7 @@
     </row>
     <row r="52" spans="2:30">
       <c r="B52" s="83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C52" s="63"/>
       <c r="D52" s="63"/>
@@ -11094,7 +11090,7 @@
     </row>
     <row r="53" spans="2:30">
       <c r="B53" s="83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C53" s="64"/>
       <c r="D53" s="64"/>
@@ -11127,7 +11123,7 @@
     </row>
     <row r="54" spans="2:30">
       <c r="B54" s="83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C54" s="63"/>
       <c r="D54" s="63"/>
@@ -11160,7 +11156,7 @@
     </row>
     <row r="55" spans="2:30">
       <c r="B55" s="83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C55" s="64"/>
       <c r="D55" s="64"/>
@@ -11193,7 +11189,7 @@
     </row>
     <row r="56" spans="2:30">
       <c r="B56" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C56" s="63"/>
       <c r="D56" s="63"/>
@@ -11226,7 +11222,7 @@
     </row>
     <row r="57" spans="2:30">
       <c r="B57" s="83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C57" s="64"/>
       <c r="D57" s="64"/>
@@ -11259,7 +11255,7 @@
     </row>
     <row r="58" spans="2:30">
       <c r="B58" s="83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C58" s="63"/>
       <c r="D58" s="63"/>
@@ -11292,7 +11288,7 @@
     </row>
     <row r="59" spans="2:30">
       <c r="B59" s="83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="64"/>
       <c r="D59" s="64"/>
@@ -11325,7 +11321,7 @@
     </row>
     <row r="60" spans="2:30">
       <c r="B60" s="83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C60" s="63"/>
       <c r="D60" s="63"/>
@@ -11358,7 +11354,7 @@
     </row>
     <row r="61" spans="2:30">
       <c r="B61" s="83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="64"/>
       <c r="D61" s="64"/>
@@ -11391,7 +11387,7 @@
     </row>
     <row r="62" spans="2:30">
       <c r="B62" s="83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="63"/>
       <c r="D62" s="63"/>
@@ -11424,7 +11420,7 @@
     </row>
     <row r="63" spans="2:30">
       <c r="B63" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C63" s="64"/>
       <c r="D63" s="64"/>
@@ -11457,7 +11453,7 @@
     </row>
     <row r="64" spans="2:30">
       <c r="B64" s="83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C64" s="63"/>
       <c r="D64" s="63"/>
@@ -11494,21 +11490,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" style="76" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" customWidth="1"/>
-    <col min="3" max="31" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" customWidth="1"/>
+    <col min="3" max="31" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="69" customFormat="1" ht="72.5">
+    <row r="1" spans="1:31" s="69" customFormat="1" ht="90">
       <c r="A1" s="40" t="s">
         <v>94</v>
       </c>
@@ -12164,7 +12160,7 @@
     </row>
     <row r="17" spans="2:31">
       <c r="B17" s="83" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="C17" s="74"/>
       <c r="D17" s="74"/>
@@ -12206,7 +12202,7 @@
     </row>
     <row r="18" spans="2:31">
       <c r="B18" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="73"/>
       <c r="D18" s="73"/>
@@ -12248,7 +12244,7 @@
     </row>
     <row r="19" spans="2:31">
       <c r="B19" s="83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="74"/>
       <c r="D19" s="74"/>
@@ -12290,7 +12286,7 @@
     </row>
     <row r="20" spans="2:31">
       <c r="B20" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="73"/>
       <c r="D20" s="73"/>
@@ -12332,7 +12328,7 @@
     </row>
     <row r="21" spans="2:31">
       <c r="B21" s="83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="74"/>
       <c r="D21" s="74"/>
@@ -12374,7 +12370,7 @@
     </row>
     <row r="22" spans="2:31">
       <c r="B22" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
@@ -12408,7 +12404,7 @@
     </row>
     <row r="23" spans="2:31">
       <c r="B23" s="83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="74"/>
       <c r="D23" s="74"/>
@@ -12446,7 +12442,7 @@
     </row>
     <row r="24" spans="2:31">
       <c r="B24" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="73"/>
@@ -12484,7 +12480,7 @@
     </row>
     <row r="25" spans="2:31">
       <c r="B25" s="83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="74"/>
       <c r="D25" s="74"/>
@@ -12522,7 +12518,7 @@
     </row>
     <row r="26" spans="2:31">
       <c r="B26" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="73"/>
       <c r="D26" s="73"/>
@@ -12556,7 +12552,7 @@
     </row>
     <row r="27" spans="2:31">
       <c r="B27" s="83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="74"/>
       <c r="D27" s="74"/>
@@ -12590,7 +12586,7 @@
     </row>
     <row r="28" spans="2:31">
       <c r="B28" s="83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="73"/>
       <c r="D28" s="73"/>
@@ -12624,7 +12620,7 @@
     </row>
     <row r="29" spans="2:31">
       <c r="B29" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="74"/>
       <c r="D29" s="74"/>
@@ -12664,7 +12660,7 @@
     </row>
     <row r="30" spans="2:31">
       <c r="B30" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C30" s="73"/>
       <c r="D30" s="73"/>
@@ -12698,7 +12694,7 @@
     </row>
     <row r="31" spans="2:31">
       <c r="B31" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C31" s="74"/>
       <c r="D31" s="74"/>
@@ -12736,7 +12732,7 @@
     </row>
     <row r="32" spans="2:31">
       <c r="B32" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="73"/>
       <c r="D32" s="73"/>
@@ -12774,7 +12770,7 @@
     </row>
     <row r="33" spans="2:31">
       <c r="B33" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="74">
         <v>0.87</v>
@@ -12812,7 +12808,7 @@
     </row>
     <row r="34" spans="2:31">
       <c r="B34" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C34" s="73">
         <v>0.87</v>
@@ -12850,7 +12846,7 @@
     </row>
     <row r="35" spans="2:31">
       <c r="B35" s="83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="74">
         <v>0.87</v>
@@ -12888,7 +12884,7 @@
     </row>
     <row r="36" spans="2:31">
       <c r="B36" s="83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C36" s="73"/>
       <c r="D36" s="73"/>
@@ -12926,7 +12922,7 @@
     </row>
     <row r="37" spans="2:31">
       <c r="B37" s="83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="74">
         <v>0.87</v>
@@ -12964,7 +12960,7 @@
     </row>
     <row r="38" spans="2:31">
       <c r="B38" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="73"/>
       <c r="D38" s="73"/>
@@ -13002,7 +12998,7 @@
     </row>
     <row r="39" spans="2:31">
       <c r="B39" s="83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C39" s="74"/>
       <c r="D39" s="74"/>
@@ -13040,7 +13036,7 @@
     </row>
     <row r="40" spans="2:31">
       <c r="B40" s="83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C40" s="73"/>
       <c r="D40" s="73"/>
@@ -13078,7 +13074,7 @@
     </row>
     <row r="41" spans="2:31">
       <c r="B41" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C41" s="74"/>
       <c r="D41" s="74"/>
@@ -13114,7 +13110,7 @@
     </row>
     <row r="42" spans="2:31">
       <c r="B42" s="83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="73"/>
       <c r="D42" s="73"/>
@@ -13150,7 +13146,7 @@
     </row>
     <row r="43" spans="2:31">
       <c r="B43" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="74"/>
       <c r="D43" s="74"/>
@@ -13184,7 +13180,7 @@
     </row>
     <row r="44" spans="2:31">
       <c r="B44" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44" s="73"/>
       <c r="D44" s="73"/>
@@ -13218,7 +13214,7 @@
     </row>
     <row r="45" spans="2:31">
       <c r="B45" s="83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="74"/>
       <c r="D45" s="74"/>
@@ -13252,7 +13248,7 @@
     </row>
     <row r="46" spans="2:31">
       <c r="B46" s="83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="73"/>
       <c r="D46" s="73"/>
@@ -13286,7 +13282,7 @@
     </row>
     <row r="47" spans="2:31">
       <c r="B47" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" s="74"/>
       <c r="D47" s="74"/>
@@ -13320,7 +13316,7 @@
     </row>
     <row r="48" spans="2:31">
       <c r="B48" s="83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48" s="73"/>
       <c r="D48" s="73"/>
@@ -13354,7 +13350,7 @@
     </row>
     <row r="49" spans="2:31">
       <c r="B49" s="83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C49" s="74"/>
       <c r="D49" s="74"/>
@@ -13388,7 +13384,7 @@
     </row>
     <row r="50" spans="2:31">
       <c r="B50" s="83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="73"/>
       <c r="D50" s="73"/>
@@ -13422,7 +13418,7 @@
     </row>
     <row r="51" spans="2:31">
       <c r="B51" s="83" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" s="74"/>
       <c r="D51" s="74"/>
@@ -13456,7 +13452,7 @@
     </row>
     <row r="52" spans="2:31">
       <c r="B52" s="83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C52" s="73"/>
       <c r="D52" s="73"/>
@@ -13490,7 +13486,7 @@
     </row>
     <row r="53" spans="2:31">
       <c r="B53" s="83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C53" s="74"/>
       <c r="D53" s="74"/>
@@ -13524,7 +13520,7 @@
     </row>
     <row r="54" spans="2:31">
       <c r="B54" s="83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C54" s="73"/>
       <c r="D54" s="73"/>
@@ -13558,7 +13554,7 @@
     </row>
     <row r="55" spans="2:31">
       <c r="B55" s="83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C55" s="74"/>
       <c r="D55" s="74"/>
@@ -13592,7 +13588,7 @@
     </row>
     <row r="56" spans="2:31">
       <c r="B56" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C56" s="73"/>
       <c r="D56" s="73"/>
@@ -13626,7 +13622,7 @@
     </row>
     <row r="57" spans="2:31">
       <c r="B57" s="83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C57" s="74"/>
       <c r="D57" s="74"/>
@@ -13660,7 +13656,7 @@
     </row>
     <row r="58" spans="2:31">
       <c r="B58" s="83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C58" s="73"/>
       <c r="D58" s="73"/>
@@ -13694,7 +13690,7 @@
     </row>
     <row r="59" spans="2:31">
       <c r="B59" s="83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="74"/>
       <c r="D59" s="74"/>
@@ -13728,7 +13724,7 @@
     </row>
     <row r="60" spans="2:31">
       <c r="B60" s="83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C60" s="73"/>
       <c r="D60" s="73"/>
@@ -13762,7 +13758,7 @@
     </row>
     <row r="61" spans="2:31">
       <c r="B61" s="83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="74"/>
       <c r="D61" s="74"/>
@@ -13796,7 +13792,7 @@
     </row>
     <row r="62" spans="2:31">
       <c r="B62" s="83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="73"/>
       <c r="D62" s="73"/>
@@ -13830,7 +13826,7 @@
     </row>
     <row r="63" spans="2:31">
       <c r="B63" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C63" s="74"/>
       <c r="D63" s="74"/>
@@ -13864,7 +13860,7 @@
     </row>
     <row r="64" spans="2:31">
       <c r="B64" s="83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C64" s="75"/>
       <c r="D64" s="75"/>
@@ -13902,21 +13898,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF70"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.1796875" style="76" customWidth="1"/>
-    <col min="2" max="2" width="49.26953125" customWidth="1"/>
-    <col min="3" max="31" width="16.26953125" customWidth="1"/>
+    <col min="1" max="1" width="65.140625" style="76" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="3" max="31" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="69" customFormat="1" ht="43.5">
+    <row r="1" spans="1:31" s="69" customFormat="1" ht="60">
       <c r="A1" s="40" t="s">
         <v>94</v>
       </c>
@@ -14554,7 +14550,7 @@
     </row>
     <row r="17" spans="2:31">
       <c r="B17" s="83" t="s">
-        <v>169</v>
+        <v>217</v>
       </c>
       <c r="C17" s="79"/>
       <c r="D17" s="79"/>
@@ -14596,7 +14592,7 @@
     </row>
     <row r="18" spans="2:31">
       <c r="B18" s="83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C18" s="78"/>
       <c r="D18" s="78"/>
@@ -14638,7 +14634,7 @@
     </row>
     <row r="19" spans="2:31">
       <c r="B19" s="83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="79"/>
       <c r="D19" s="79"/>
@@ -14680,7 +14676,7 @@
     </row>
     <row r="20" spans="2:31">
       <c r="B20" s="83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
@@ -14722,7 +14718,7 @@
     </row>
     <row r="21" spans="2:31">
       <c r="B21" s="83" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="79"/>
       <c r="D21" s="79"/>
@@ -14764,7 +14760,7 @@
     </row>
     <row r="22" spans="2:31">
       <c r="B22" s="83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C22" s="78"/>
       <c r="D22" s="78"/>
@@ -14798,7 +14794,7 @@
     </row>
     <row r="23" spans="2:31">
       <c r="B23" s="83" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C23" s="79"/>
       <c r="D23" s="79"/>
@@ -14836,7 +14832,7 @@
     </row>
     <row r="24" spans="2:31">
       <c r="B24" s="83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="78"/>
       <c r="D24" s="78"/>
@@ -14874,7 +14870,7 @@
     </row>
     <row r="25" spans="2:31">
       <c r="B25" s="83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C25" s="79"/>
       <c r="D25" s="79"/>
@@ -14912,7 +14908,7 @@
     </row>
     <row r="26" spans="2:31">
       <c r="B26" s="83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C26" s="78"/>
       <c r="D26" s="78"/>
@@ -14946,7 +14942,7 @@
     </row>
     <row r="27" spans="2:31">
       <c r="B27" s="83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="79"/>
       <c r="D27" s="79"/>
@@ -14980,7 +14976,7 @@
     </row>
     <row r="28" spans="2:31">
       <c r="B28" s="83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="78"/>
       <c r="D28" s="78"/>
@@ -15014,7 +15010,7 @@
     </row>
     <row r="29" spans="2:31">
       <c r="B29" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="79"/>
       <c r="D29" s="79"/>
@@ -15054,7 +15050,7 @@
     </row>
     <row r="30" spans="2:31">
       <c r="B30" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C30" s="78"/>
       <c r="D30" s="78"/>
@@ -15088,7 +15084,7 @@
     </row>
     <row r="31" spans="2:31">
       <c r="B31" s="83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C31" s="79"/>
       <c r="D31" s="79"/>
@@ -15126,7 +15122,7 @@
     </row>
     <row r="32" spans="2:31">
       <c r="B32" s="83" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="78"/>
@@ -15164,7 +15160,7 @@
     </row>
     <row r="33" spans="2:31">
       <c r="B33" s="83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C33" s="79">
         <v>0.94</v>
@@ -15202,7 +15198,7 @@
     </row>
     <row r="34" spans="2:31">
       <c r="B34" s="83" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C34" s="78">
         <v>0.94</v>
@@ -15240,7 +15236,7 @@
     </row>
     <row r="35" spans="2:31">
       <c r="B35" s="83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C35" s="79">
         <v>0.94</v>
@@ -15278,7 +15274,7 @@
     </row>
     <row r="36" spans="2:31">
       <c r="B36" s="83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C36" s="78"/>
       <c r="D36" s="78"/>
@@ -15316,7 +15312,7 @@
     </row>
     <row r="37" spans="2:31">
       <c r="B37" s="83" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="79">
         <v>0.94</v>
@@ -15354,7 +15350,7 @@
     </row>
     <row r="38" spans="2:31">
       <c r="B38" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="78"/>
       <c r="D38" s="78"/>
@@ -15392,7 +15388,7 @@
     </row>
     <row r="39" spans="2:31">
       <c r="B39" s="83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C39" s="79"/>
       <c r="D39" s="79"/>
@@ -15430,7 +15426,7 @@
     </row>
     <row r="40" spans="2:31">
       <c r="B40" s="83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C40" s="78"/>
       <c r="D40" s="78"/>
@@ -15468,7 +15464,7 @@
     </row>
     <row r="41" spans="2:31">
       <c r="B41" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C41" s="79"/>
       <c r="D41" s="79"/>
@@ -15504,7 +15500,7 @@
     </row>
     <row r="42" spans="2:31">
       <c r="B42" s="83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C42" s="78"/>
       <c r="D42" s="78"/>
@@ -15540,7 +15536,7 @@
     </row>
     <row r="43" spans="2:31">
       <c r="B43" s="83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="79"/>
       <c r="D43" s="79"/>
@@ -15574,7 +15570,7 @@
     </row>
     <row r="44" spans="2:31">
       <c r="B44" s="83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C44" s="78"/>
       <c r="D44" s="78"/>
@@ -15608,7 +15604,7 @@
     </row>
     <row r="45" spans="2:31">
       <c r="B45" s="83" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="79"/>
       <c r="D45" s="79"/>
@@ -15642,7 +15638,7 @@
     </row>
     <row r="46" spans="2:31">
       <c r="B46" s="83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="78"/>
       <c r="D46" s="78"/>
@@ -15676,7 +15672,7 @@
     </row>
     <row r="47" spans="2:31">
       <c r="B47" s="83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C47" s="79"/>
       <c r="D47" s="79"/>
@@ -15710,7 +15706,7 @@
     </row>
     <row r="48" spans="2:31">
       <c r="B48" s="83" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48" s="78"/>
       <c r="D48" s="78"/>
@@ -15744,7 +15740,7 @@
     </row>
     <row r="49" spans="2:31">
       <c r="B49" s="83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C49" s="79"/>
       <c r="D49" s="79"/>
@@ -15778,7 +15774,7 @@
     </row>
     <row r="50" spans="2:31">
       <c r="B50" s="83" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="78"/>
       <c r="D50" s="78"/>
@@ -15812,7 +15808,7 @@
     </row>
     <row r="51" spans="2:31">
       <c r="B51" s="83" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" s="79"/>
       <c r="D51" s="79"/>
@@ -15846,7 +15842,7 @@
     </row>
     <row r="52" spans="2:31">
       <c r="B52" s="83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C52" s="78"/>
       <c r="D52" s="78"/>
@@ -15880,7 +15876,7 @@
     </row>
     <row r="53" spans="2:31">
       <c r="B53" s="83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C53" s="79"/>
       <c r="D53" s="79"/>
@@ -15914,7 +15910,7 @@
     </row>
     <row r="54" spans="2:31">
       <c r="B54" s="83" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C54" s="78"/>
       <c r="D54" s="78"/>
@@ -15948,7 +15944,7 @@
     </row>
     <row r="55" spans="2:31">
       <c r="B55" s="83" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C55" s="79"/>
       <c r="D55" s="79"/>
@@ -15982,7 +15978,7 @@
     </row>
     <row r="56" spans="2:31">
       <c r="B56" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C56" s="78"/>
       <c r="D56" s="78"/>
@@ -16016,7 +16012,7 @@
     </row>
     <row r="57" spans="2:31">
       <c r="B57" s="83" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C57" s="79"/>
       <c r="D57" s="79"/>
@@ -16050,7 +16046,7 @@
     </row>
     <row r="58" spans="2:31">
       <c r="B58" s="83" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C58" s="78"/>
       <c r="D58" s="78"/>
@@ -16084,7 +16080,7 @@
     </row>
     <row r="59" spans="2:31">
       <c r="B59" s="83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="79"/>
       <c r="D59" s="79"/>
@@ -16118,7 +16114,7 @@
     </row>
     <row r="60" spans="2:31">
       <c r="B60" s="83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C60" s="78"/>
       <c r="D60" s="78"/>
@@ -16152,7 +16148,7 @@
     </row>
     <row r="61" spans="2:31">
       <c r="B61" s="83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="79"/>
       <c r="D61" s="79"/>
@@ -16186,7 +16182,7 @@
     </row>
     <row r="62" spans="2:31">
       <c r="B62" s="83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="78"/>
       <c r="D62" s="78"/>
@@ -16220,7 +16216,7 @@
     </row>
     <row r="63" spans="2:31">
       <c r="B63" s="83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C63" s="79"/>
       <c r="D63" s="79"/>
@@ -16254,7 +16250,7 @@
     </row>
     <row r="64" spans="2:31">
       <c r="B64" s="83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C64" s="80"/>
       <c r="D64" s="80"/>

</xml_diff>

<commit_message>
New composting + class for flow and processes
</commit_message>
<xml_diff>
--- a/Material properties - process modles.xlsx
+++ b/Material properties - process modles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="6"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Composting" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="223">
   <si>
     <t>Substrate mass flows inputs</t>
   </si>
@@ -684,6 +684,21 @@
   </si>
   <si>
     <t>Magazines</t>
+  </si>
+  <si>
+    <t>Percent of Generated Methane used for Energy</t>
+  </si>
+  <si>
+    <t>Percent of Generated Methane oxidized</t>
+  </si>
+  <si>
+    <t>Percent of Generated Methane Emitted</t>
+  </si>
+  <si>
+    <t>Percent of Generated Methane Flared</t>
+  </si>
+  <si>
+    <t>LF model</t>
   </si>
 </sst>
 </file>
@@ -972,7 +987,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1214,6 +1229,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1545,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O1" sqref="L1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1556,14 +1584,16 @@
     <col min="1" max="1" width="26.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="25.5703125" style="19" customWidth="1"/>
-    <col min="14" max="14" width="31" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="63" width="25.5703125" style="19" customWidth="1"/>
-    <col min="64" max="16384" width="9.140625" style="19"/>
+    <col min="4" max="11" width="25.5703125" style="19" customWidth="1"/>
+    <col min="12" max="15" width="25.5703125" style="58" customWidth="1"/>
+    <col min="16" max="17" width="25.5703125" style="19" customWidth="1"/>
+    <col min="18" max="18" width="31" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="67" width="25.5703125" style="19" customWidth="1"/>
+    <col min="68" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" ht="81" customHeight="1">
+    <row r="1" spans="1:19" s="16" customFormat="1" ht="81" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1597,18 +1627,30 @@
       <c r="K1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="23" t="s">
+      <c r="L1" s="90" t="s">
+        <v>218</v>
+      </c>
+      <c r="M1" s="90" t="s">
+        <v>219</v>
+      </c>
+      <c r="N1" s="90" t="s">
+        <v>220</v>
+      </c>
+      <c r="O1" s="90" t="s">
+        <v>221</v>
+      </c>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="15" t="s">
+      <c r="R1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:19">
       <c r="A2" s="8"/>
       <c r="B2" s="17" t="s">
         <v>2</v>
@@ -1630,16 +1672,28 @@
         <v>70</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="17" t="s">
+      <c r="L2" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="M2" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="N2" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="O2" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:19">
       <c r="A3" s="8"/>
       <c r="B3" s="20" t="s">
         <v>3</v>
@@ -1671,16 +1725,28 @@
       <c r="K3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="20" t="s">
+      <c r="L3" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="S3" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="58" customFormat="1">
+    <row r="4" spans="1:19" s="58" customFormat="1">
       <c r="A4" s="8"/>
       <c r="B4" s="20" t="s">
         <v>82</v>
@@ -1694,12 +1760,16 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="21"/>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="21"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="8"/>
       <c r="B5" s="83" t="s">
         <v>160</v>
@@ -1731,14 +1801,26 @@
       <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="20" t="s">
+      <c r="L5" s="89">
+        <v>40.453667103041987</v>
+      </c>
+      <c r="M5" s="89">
+        <v>3.8551462933222229</v>
+      </c>
+      <c r="N5" s="87">
+        <v>26.942537613293517</v>
+      </c>
+      <c r="O5" s="87">
+        <v>28.748648990342275</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="9"/>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="8"/>
       <c r="B6" s="83" t="s">
         <v>161</v>
@@ -1770,14 +1852,26 @@
       <c r="K6" s="9">
         <v>1</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="20" t="s">
+      <c r="L6" s="89">
+        <v>24.20655340611955</v>
+      </c>
+      <c r="M6" s="89">
+        <v>4.2099176569894787</v>
+      </c>
+      <c r="N6" s="87">
+        <v>33.503697246598598</v>
+      </c>
+      <c r="O6" s="87">
+        <v>38.079831690292373</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="8"/>
       <c r="B7" s="83" t="s">
         <v>162</v>
@@ -1809,14 +1903,26 @@
       <c r="K7" s="9">
         <v>1</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="20" t="s">
+      <c r="L7" s="89">
+        <v>37.922310101343321</v>
+      </c>
+      <c r="M7" s="89">
+        <v>16.894724535937865</v>
+      </c>
+      <c r="N7" s="87">
+        <v>38.969241119370921</v>
+      </c>
+      <c r="O7" s="87">
+        <v>6.2137242433478974</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="9"/>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="8"/>
       <c r="B8" s="83" t="s">
         <v>163</v>
@@ -1848,14 +1954,26 @@
       <c r="K8" s="9">
         <v>1</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="20" t="s">
+      <c r="L8" s="89">
+        <v>44.563130721438888</v>
+      </c>
+      <c r="M8" s="89">
+        <v>3.9864523347987388</v>
+      </c>
+      <c r="N8" s="87">
+        <v>25.613545462343208</v>
+      </c>
+      <c r="O8" s="87">
+        <v>25.836871481419166</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="9"/>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="8"/>
       <c r="B9" s="83" t="s">
         <v>164</v>
@@ -1887,14 +2005,26 @@
       <c r="K9" s="9">
         <v>1</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="20" t="s">
+      <c r="L9" s="89">
+        <v>44.563130721438853</v>
+      </c>
+      <c r="M9" s="89">
+        <v>3.9864523347987366</v>
+      </c>
+      <c r="N9" s="87">
+        <v>25.613545462343168</v>
+      </c>
+      <c r="O9" s="87">
+        <v>25.836871481419251</v>
+      </c>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="8"/>
       <c r="B10" s="83" t="s">
         <v>9</v>
@@ -1926,14 +2056,26 @@
       <c r="K10" s="9">
         <v>1</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="20" t="s">
+      <c r="L10" s="89">
+        <v>51.156662692132173</v>
+      </c>
+      <c r="M10" s="89">
+        <v>7.8841320437625262</v>
+      </c>
+      <c r="N10" s="87">
+        <v>26.799770977154484</v>
+      </c>
+      <c r="O10" s="87">
+        <v>14.159434286950813</v>
+      </c>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="3"/>
       <c r="B11" s="83" t="s">
         <v>165</v>
@@ -1965,14 +2107,26 @@
       <c r="K11" s="9">
         <v>1</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="20" t="s">
+      <c r="L11" s="89">
+        <v>51.156662692132194</v>
+      </c>
+      <c r="M11" s="89">
+        <v>7.8841320437625289</v>
+      </c>
+      <c r="N11" s="87">
+        <v>26.799770977154502</v>
+      </c>
+      <c r="O11" s="87">
+        <v>14.159434286950784</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="3"/>
       <c r="B12" s="83" t="s">
         <v>11</v>
@@ -2004,14 +2158,26 @@
       <c r="K12" s="9">
         <v>1</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="20" t="s">
+      <c r="L12" s="89">
+        <v>44.027727796234672</v>
+      </c>
+      <c r="M12" s="89">
+        <v>13.453599157505661</v>
+      </c>
+      <c r="N12" s="87">
+        <v>33.979895620423065</v>
+      </c>
+      <c r="O12" s="87">
+        <v>8.5387774258365994</v>
+      </c>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="8"/>
       <c r="B13" s="83" t="s">
         <v>166</v>
@@ -2043,14 +2209,26 @@
       <c r="K13" s="9">
         <v>0</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="20" t="s">
+      <c r="L13" s="89">
+        <v>0</v>
+      </c>
+      <c r="M13" s="89">
+        <v>0</v>
+      </c>
+      <c r="N13" s="87">
+        <v>0</v>
+      </c>
+      <c r="O13" s="87">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="8"/>
       <c r="B14" s="83" t="s">
         <v>13</v>
@@ -2082,14 +2260,26 @@
       <c r="K14" s="9">
         <v>1</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="20" t="s">
+      <c r="L14" s="89">
+        <v>45.254686949269271</v>
+      </c>
+      <c r="M14" s="89">
+        <v>12.692129498156582</v>
+      </c>
+      <c r="N14" s="87">
+        <v>32.917259248276224</v>
+      </c>
+      <c r="O14" s="87">
+        <v>9.1359243042979301</v>
+      </c>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="8"/>
       <c r="B15" s="83" t="s">
         <v>167</v>
@@ -2121,14 +2311,26 @@
       <c r="K15" s="9">
         <v>1</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="20" t="s">
+      <c r="L15" s="89">
+        <v>40.060402076129378</v>
+      </c>
+      <c r="M15" s="89">
+        <v>15.740031149967967</v>
+      </c>
+      <c r="N15" s="87">
+        <v>37.264467670202784</v>
+      </c>
+      <c r="O15" s="87">
+        <v>6.9350991036998693</v>
+      </c>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="8"/>
       <c r="B16" s="83" t="s">
         <v>168</v>
@@ -2160,14 +2362,26 @@
       <c r="K16" s="9">
         <v>1</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="20" t="s">
+      <c r="L16" s="89">
+        <v>44.027727796234686</v>
+      </c>
+      <c r="M16" s="89">
+        <v>13.453599157505661</v>
+      </c>
+      <c r="N16" s="87">
+        <v>33.979895620423065</v>
+      </c>
+      <c r="O16" s="87">
+        <v>8.5387774258365852</v>
+      </c>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="O16" s="9"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="8"/>
       <c r="B17" s="83" t="s">
         <v>217</v>
@@ -2199,14 +2413,26 @@
       <c r="K17" s="9">
         <v>1</v>
       </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="20" t="s">
+      <c r="L17" s="89">
+        <v>47.8240101290599</v>
+      </c>
+      <c r="M17" s="89">
+        <v>4.3160275423909011</v>
+      </c>
+      <c r="N17" s="87">
+        <v>24.785614004914009</v>
+      </c>
+      <c r="O17" s="87">
+        <v>23.074348323635192</v>
+      </c>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="9"/>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="S17" s="9"/>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="8"/>
       <c r="B18" s="83" t="s">
         <v>169</v>
@@ -2238,14 +2464,26 @@
       <c r="K18" s="9">
         <v>1</v>
       </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="20" t="s">
+      <c r="L18" s="89">
+        <v>47.824010129059872</v>
+      </c>
+      <c r="M18" s="89">
+        <v>4.3160275423908985</v>
+      </c>
+      <c r="N18" s="87">
+        <v>24.785614004914009</v>
+      </c>
+      <c r="O18" s="87">
+        <v>23.07434832363522</v>
+      </c>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="9"/>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="8"/>
       <c r="B19" s="83" t="s">
         <v>170</v>
@@ -2277,14 +2515,26 @@
       <c r="K19" s="9">
         <v>1</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="20" t="s">
+      <c r="L19" s="89">
+        <v>40.060402076129392</v>
+      </c>
+      <c r="M19" s="89">
+        <v>15.740031149967976</v>
+      </c>
+      <c r="N19" s="87">
+        <v>37.264467670202784</v>
+      </c>
+      <c r="O19" s="87">
+        <v>6.935099103699855</v>
+      </c>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="O19" s="9"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="S19" s="9"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="8"/>
       <c r="B20" s="83" t="s">
         <v>171</v>
@@ -2316,14 +2566,26 @@
       <c r="K20" s="9">
         <v>1</v>
       </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="20" t="s">
+      <c r="L20" s="89">
+        <v>40.060402076129371</v>
+      </c>
+      <c r="M20" s="89">
+        <v>15.740031149967971</v>
+      </c>
+      <c r="N20" s="87">
+        <v>37.264467670202784</v>
+      </c>
+      <c r="O20" s="87">
+        <v>6.9350991036998835</v>
+      </c>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="S20" s="9"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="8"/>
       <c r="B21" s="83" t="s">
         <v>172</v>
@@ -2355,14 +2617,26 @@
       <c r="K21" s="9">
         <v>1</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="20" t="s">
+      <c r="L21" s="89">
+        <v>44.671577518796205</v>
+      </c>
+      <c r="M21" s="89">
+        <v>13.058173881020064</v>
+      </c>
+      <c r="N21" s="87">
+        <v>33.425889852467733</v>
+      </c>
+      <c r="O21" s="87">
+        <v>8.8443587477160008</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="S21" s="9"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="8"/>
       <c r="B22" s="83" t="s">
         <v>173</v>
@@ -2394,14 +2668,26 @@
       <c r="K22" s="9">
         <v>1</v>
       </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="20" t="s">
+      <c r="L22" s="89">
+        <v>47.82401012905985</v>
+      </c>
+      <c r="M22" s="89">
+        <v>4.3160275423909003</v>
+      </c>
+      <c r="N22" s="87">
+        <v>24.785614004913992</v>
+      </c>
+      <c r="O22" s="87">
+        <v>23.074348323635263</v>
+      </c>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="O22" s="9"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="S22" s="9"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="8"/>
       <c r="B23" s="83" t="s">
         <v>174</v>
@@ -2433,14 +2719,26 @@
       <c r="K23" s="9">
         <v>0</v>
       </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="20" t="s">
+      <c r="L23" s="89">
+        <v>0</v>
+      </c>
+      <c r="M23" s="89">
+        <v>0</v>
+      </c>
+      <c r="N23" s="87">
+        <v>0</v>
+      </c>
+      <c r="O23" s="87">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="S23" s="9"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="8"/>
       <c r="B24" s="83" t="s">
         <v>175</v>
@@ -2472,14 +2770,26 @@
       <c r="K24" s="9">
         <v>0</v>
       </c>
-      <c r="L24" s="1"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="20" t="s">
+      <c r="L24" s="89">
+        <v>0</v>
+      </c>
+      <c r="M24" s="89">
+        <v>0</v>
+      </c>
+      <c r="N24" s="87">
+        <v>0</v>
+      </c>
+      <c r="O24" s="87">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="O24" s="9"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="S24" s="9"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="8"/>
       <c r="B25" s="83" t="s">
         <v>176</v>
@@ -2511,14 +2821,26 @@
       <c r="K25" s="9">
         <v>0</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="20" t="s">
+      <c r="L25" s="89">
+        <v>0</v>
+      </c>
+      <c r="M25" s="89">
+        <v>0</v>
+      </c>
+      <c r="N25" s="87">
+        <v>0</v>
+      </c>
+      <c r="O25" s="87">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="O25" s="9"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="S25" s="9"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="8"/>
       <c r="B26" s="83" t="s">
         <v>177</v>
@@ -2550,14 +2872,26 @@
       <c r="K26" s="9">
         <v>0</v>
       </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="20" t="s">
+      <c r="L26" s="89">
+        <v>0</v>
+      </c>
+      <c r="M26" s="89">
+        <v>0</v>
+      </c>
+      <c r="N26" s="87">
+        <v>0</v>
+      </c>
+      <c r="O26" s="87">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="9"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="S26" s="9"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="8"/>
       <c r="B27" s="83" t="s">
         <v>178</v>
@@ -2589,14 +2923,26 @@
       <c r="K27" s="9">
         <v>0</v>
       </c>
-      <c r="L27" s="1"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="20" t="s">
+      <c r="L27" s="89">
+        <v>0</v>
+      </c>
+      <c r="M27" s="89">
+        <v>0</v>
+      </c>
+      <c r="N27" s="87">
+        <v>0</v>
+      </c>
+      <c r="O27" s="87">
+        <v>0</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="O27" s="9"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="S27" s="9"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="8"/>
       <c r="B28" s="83" t="s">
         <v>179</v>
@@ -2628,14 +2974,26 @@
       <c r="K28" s="9">
         <v>0</v>
       </c>
-      <c r="L28" s="1"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="20" t="s">
+      <c r="L28" s="89">
+        <v>0</v>
+      </c>
+      <c r="M28" s="89">
+        <v>0</v>
+      </c>
+      <c r="N28" s="87">
+        <v>0</v>
+      </c>
+      <c r="O28" s="87">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="O28" s="9"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="S28" s="9"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="8"/>
       <c r="B29" s="83" t="s">
         <v>180</v>
@@ -2667,14 +3025,26 @@
       <c r="K29" s="9">
         <v>0</v>
       </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="20" t="s">
+      <c r="L29" s="89">
+        <v>0</v>
+      </c>
+      <c r="M29" s="89">
+        <v>0</v>
+      </c>
+      <c r="N29" s="87">
+        <v>0</v>
+      </c>
+      <c r="O29" s="87">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O29" s="9"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="S29" s="9"/>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="8"/>
       <c r="B30" s="83" t="s">
         <v>181</v>
@@ -2706,14 +3076,26 @@
       <c r="K30" s="9">
         <v>0</v>
       </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="20" t="s">
+      <c r="L30" s="89">
+        <v>0</v>
+      </c>
+      <c r="M30" s="89">
+        <v>0</v>
+      </c>
+      <c r="N30" s="87">
+        <v>0</v>
+      </c>
+      <c r="O30" s="87">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="O30" s="9"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="S30" s="9"/>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="8"/>
       <c r="B31" s="83" t="s">
         <v>182</v>
@@ -2745,14 +3127,26 @@
       <c r="K31" s="9">
         <v>0</v>
       </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="20" t="s">
+      <c r="L31" s="89">
+        <v>0</v>
+      </c>
+      <c r="M31" s="89">
+        <v>0</v>
+      </c>
+      <c r="N31" s="87">
+        <v>0</v>
+      </c>
+      <c r="O31" s="87">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="O31" s="9"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="S31" s="9"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="8"/>
       <c r="B32" s="83" t="s">
         <v>183</v>
@@ -2784,14 +3178,26 @@
       <c r="K32" s="9">
         <v>0</v>
       </c>
-      <c r="L32" s="1"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="20" t="s">
+      <c r="L32" s="89">
+        <v>0</v>
+      </c>
+      <c r="M32" s="89">
+        <v>0</v>
+      </c>
+      <c r="N32" s="87">
+        <v>0</v>
+      </c>
+      <c r="O32" s="87">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="O32" s="9"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="S32" s="9"/>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="8"/>
       <c r="B33" s="83" t="s">
         <v>184</v>
@@ -2823,14 +3229,26 @@
       <c r="K33" s="9">
         <v>0</v>
       </c>
-      <c r="L33" s="1"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="20" t="s">
+      <c r="L33" s="89">
+        <v>0</v>
+      </c>
+      <c r="M33" s="89">
+        <v>0</v>
+      </c>
+      <c r="N33" s="87">
+        <v>0</v>
+      </c>
+      <c r="O33" s="87">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="O33" s="9"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="S33" s="9"/>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="8"/>
       <c r="B34" s="83" t="s">
         <v>185</v>
@@ -2862,14 +3280,26 @@
       <c r="K34" s="9">
         <v>0</v>
       </c>
-      <c r="L34" s="1"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="20" t="s">
+      <c r="L34" s="89">
+        <v>0</v>
+      </c>
+      <c r="M34" s="89">
+        <v>0</v>
+      </c>
+      <c r="N34" s="87">
+        <v>0</v>
+      </c>
+      <c r="O34" s="87">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="O34" s="9"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="S34" s="9"/>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="8"/>
       <c r="B35" s="83" t="s">
         <v>186</v>
@@ -2901,14 +3331,26 @@
       <c r="K35" s="9">
         <v>0</v>
       </c>
-      <c r="L35" s="1"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="20" t="s">
+      <c r="L35" s="89">
+        <v>0</v>
+      </c>
+      <c r="M35" s="89">
+        <v>0</v>
+      </c>
+      <c r="N35" s="87">
+        <v>0</v>
+      </c>
+      <c r="O35" s="87">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="O35" s="9"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="S35" s="9"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="8"/>
       <c r="B36" s="83" t="s">
         <v>187</v>
@@ -2940,14 +3382,26 @@
       <c r="K36" s="9">
         <v>0</v>
       </c>
-      <c r="L36" s="1"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="20" t="s">
+      <c r="L36" s="89">
+        <v>0</v>
+      </c>
+      <c r="M36" s="89">
+        <v>0</v>
+      </c>
+      <c r="N36" s="87">
+        <v>0</v>
+      </c>
+      <c r="O36" s="87">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="O36" s="9"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="S36" s="9"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="8"/>
       <c r="B37" s="83" t="s">
         <v>188</v>
@@ -2979,14 +3433,26 @@
       <c r="K37" s="9">
         <v>0</v>
       </c>
-      <c r="L37" s="1"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="20" t="s">
+      <c r="L37" s="89">
+        <v>0</v>
+      </c>
+      <c r="M37" s="89">
+        <v>0</v>
+      </c>
+      <c r="N37" s="87">
+        <v>0</v>
+      </c>
+      <c r="O37" s="87">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="O37" s="9"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="S37" s="9"/>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="8"/>
       <c r="B38" s="83" t="s">
         <v>189</v>
@@ -3018,14 +3484,26 @@
       <c r="K38" s="9">
         <v>0</v>
       </c>
-      <c r="L38" s="1"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="20" t="s">
+      <c r="L38" s="89">
+        <v>0</v>
+      </c>
+      <c r="M38" s="89">
+        <v>0</v>
+      </c>
+      <c r="N38" s="87">
+        <v>0</v>
+      </c>
+      <c r="O38" s="87">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="O38" s="9"/>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="S38" s="9"/>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="8"/>
       <c r="B39" s="83" t="s">
         <v>190</v>
@@ -3057,14 +3535,26 @@
       <c r="K39" s="9">
         <v>0</v>
       </c>
-      <c r="L39" s="1"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="20" t="s">
+      <c r="L39" s="89">
+        <v>0</v>
+      </c>
+      <c r="M39" s="89">
+        <v>0</v>
+      </c>
+      <c r="N39" s="87">
+        <v>0</v>
+      </c>
+      <c r="O39" s="87">
+        <v>0</v>
+      </c>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="O39" s="9"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="S39" s="9"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="8"/>
       <c r="B40" s="83" t="s">
         <v>191</v>
@@ -3096,14 +3586,26 @@
       <c r="K40" s="9">
         <v>0</v>
       </c>
-      <c r="L40" s="1"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="20" t="s">
+      <c r="L40" s="89">
+        <v>0</v>
+      </c>
+      <c r="M40" s="89">
+        <v>0</v>
+      </c>
+      <c r="N40" s="87">
+        <v>0</v>
+      </c>
+      <c r="O40" s="87">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="O40" s="9"/>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="S40" s="9"/>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="8"/>
       <c r="B41" s="83" t="s">
         <v>192</v>
@@ -3135,14 +3637,26 @@
       <c r="K41" s="9">
         <v>0</v>
       </c>
-      <c r="L41" s="1"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="20" t="s">
+      <c r="L41" s="89">
+        <v>0</v>
+      </c>
+      <c r="M41" s="89">
+        <v>0</v>
+      </c>
+      <c r="N41" s="87">
+        <v>0</v>
+      </c>
+      <c r="O41" s="87">
+        <v>0</v>
+      </c>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O41" s="9"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="S41" s="9"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="8"/>
       <c r="B42" s="83" t="s">
         <v>193</v>
@@ -3174,14 +3688,26 @@
       <c r="K42" s="9">
         <v>0</v>
       </c>
-      <c r="L42" s="1"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="20" t="s">
+      <c r="L42" s="89">
+        <v>0</v>
+      </c>
+      <c r="M42" s="89">
+        <v>0</v>
+      </c>
+      <c r="N42" s="87">
+        <v>0</v>
+      </c>
+      <c r="O42" s="87">
+        <v>0</v>
+      </c>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="O42" s="9"/>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="S42" s="9"/>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="8"/>
       <c r="B43" s="83" t="s">
         <v>194</v>
@@ -3213,14 +3739,26 @@
       <c r="K43" s="9">
         <v>1</v>
       </c>
-      <c r="L43" s="1"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="20" t="s">
+      <c r="L43" s="89">
+        <v>51.265859991640617</v>
+      </c>
+      <c r="M43" s="89">
+        <v>5.5695962486522026</v>
+      </c>
+      <c r="N43" s="87">
+        <v>24.73507248608006</v>
+      </c>
+      <c r="O43" s="87">
+        <v>18.429471273627115</v>
+      </c>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="O43" s="9"/>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="S43" s="9"/>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="8"/>
       <c r="B44" s="83" t="s">
         <v>195</v>
@@ -3252,14 +3790,26 @@
       <c r="K44" s="9">
         <v>0</v>
       </c>
-      <c r="L44" s="1"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="20" t="s">
+      <c r="L44" s="89">
+        <v>0</v>
+      </c>
+      <c r="M44" s="89">
+        <v>0</v>
+      </c>
+      <c r="N44" s="87">
+        <v>0</v>
+      </c>
+      <c r="O44" s="87">
+        <v>0</v>
+      </c>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="O44" s="9"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="S44" s="9"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="8"/>
       <c r="B45" s="83" t="s">
         <v>196</v>
@@ -3291,14 +3841,26 @@
       <c r="K45" s="9">
         <v>0</v>
       </c>
-      <c r="L45" s="1"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="20" t="s">
+      <c r="L45" s="89">
+        <v>0</v>
+      </c>
+      <c r="M45" s="89">
+        <v>0</v>
+      </c>
+      <c r="N45" s="87">
+        <v>0</v>
+      </c>
+      <c r="O45" s="87">
+        <v>0</v>
+      </c>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="O45" s="9"/>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="S45" s="9"/>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="8"/>
       <c r="B46" s="83" t="s">
         <v>197</v>
@@ -3330,14 +3892,26 @@
       <c r="K46" s="9">
         <v>0</v>
       </c>
-      <c r="L46" s="1"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="20" t="s">
+      <c r="L46" s="89">
+        <v>0</v>
+      </c>
+      <c r="M46" s="89">
+        <v>0</v>
+      </c>
+      <c r="N46" s="87">
+        <v>0</v>
+      </c>
+      <c r="O46" s="87">
+        <v>0</v>
+      </c>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="O46" s="9"/>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="S46" s="9"/>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="8"/>
       <c r="B47" s="83" t="s">
         <v>198</v>
@@ -3369,14 +3943,26 @@
       <c r="K47" s="9">
         <v>0</v>
       </c>
-      <c r="L47" s="1"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="20" t="s">
+      <c r="L47" s="89">
+        <v>0</v>
+      </c>
+      <c r="M47" s="89">
+        <v>0</v>
+      </c>
+      <c r="N47" s="87">
+        <v>0</v>
+      </c>
+      <c r="O47" s="87">
+        <v>0</v>
+      </c>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="O47" s="9"/>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="S47" s="9"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="8"/>
       <c r="B48" s="83" t="s">
         <v>199</v>
@@ -3408,14 +3994,26 @@
       <c r="K48" s="9">
         <v>0</v>
       </c>
-      <c r="L48" s="1"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="20" t="s">
+      <c r="L48" s="89">
+        <v>0</v>
+      </c>
+      <c r="M48" s="89">
+        <v>0</v>
+      </c>
+      <c r="N48" s="87">
+        <v>0</v>
+      </c>
+      <c r="O48" s="87">
+        <v>0</v>
+      </c>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="O48" s="9"/>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="S48" s="9"/>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="8"/>
       <c r="B49" s="83" t="s">
         <v>200</v>
@@ -3447,14 +4045,26 @@
       <c r="K49" s="9">
         <v>0</v>
       </c>
-      <c r="L49" s="1"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="20" t="s">
+      <c r="L49" s="89">
+        <v>0</v>
+      </c>
+      <c r="M49" s="89">
+        <v>0</v>
+      </c>
+      <c r="N49" s="87">
+        <v>0</v>
+      </c>
+      <c r="O49" s="87">
+        <v>0</v>
+      </c>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="O49" s="9"/>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="S49" s="9"/>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="8"/>
       <c r="B50" s="83" t="s">
         <v>201</v>
@@ -3486,14 +4096,26 @@
       <c r="K50" s="9">
         <v>0</v>
       </c>
-      <c r="L50" s="2"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="20" t="s">
+      <c r="L50" s="89">
+        <v>44.027727796234686</v>
+      </c>
+      <c r="M50" s="89">
+        <v>13.453599157505671</v>
+      </c>
+      <c r="N50" s="87">
+        <v>33.979895620423086</v>
+      </c>
+      <c r="O50" s="87">
+        <v>8.5387774258365567</v>
+      </c>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="O50" s="9"/>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="S50" s="9"/>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="8"/>
       <c r="B51" s="83" t="s">
         <v>202</v>
@@ -3525,14 +4147,26 @@
       <c r="K51" s="9">
         <v>0</v>
       </c>
-      <c r="L51" s="2"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="20" t="s">
+      <c r="L51" s="89">
+        <v>0</v>
+      </c>
+      <c r="M51" s="89">
+        <v>0</v>
+      </c>
+      <c r="N51" s="87">
+        <v>0</v>
+      </c>
+      <c r="O51" s="87">
+        <v>0</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="8"/>
+      <c r="R51" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="O51" s="9"/>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="S51" s="9"/>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="8"/>
       <c r="B52" s="83" t="s">
         <v>203</v>
@@ -3564,14 +4198,26 @@
       <c r="K52" s="9">
         <v>0</v>
       </c>
-      <c r="L52" s="2"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="20" t="s">
+      <c r="L52" s="89">
+        <v>0</v>
+      </c>
+      <c r="M52" s="89">
+        <v>0</v>
+      </c>
+      <c r="N52" s="87">
+        <v>0</v>
+      </c>
+      <c r="O52" s="87">
+        <v>0</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="O52" s="9"/>
-    </row>
-    <row r="53" spans="1:15">
+      <c r="S52" s="9"/>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="8"/>
       <c r="B53" s="83" t="s">
         <v>204</v>
@@ -3603,14 +4249,26 @@
       <c r="K53" s="9">
         <v>0</v>
       </c>
-      <c r="L53" s="2"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="20" t="s">
+      <c r="L53" s="89">
+        <v>0</v>
+      </c>
+      <c r="M53" s="89">
+        <v>0</v>
+      </c>
+      <c r="N53" s="87">
+        <v>0</v>
+      </c>
+      <c r="O53" s="87">
+        <v>0</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="O53" s="9"/>
-    </row>
-    <row r="54" spans="1:15">
+      <c r="S53" s="9"/>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="8"/>
       <c r="B54" s="83" t="s">
         <v>205</v>
@@ -3642,14 +4300,26 @@
       <c r="K54" s="9">
         <v>0</v>
       </c>
-      <c r="L54" s="2"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="20" t="s">
+      <c r="L54" s="89">
+        <v>0</v>
+      </c>
+      <c r="M54" s="89">
+        <v>0</v>
+      </c>
+      <c r="N54" s="87">
+        <v>0</v>
+      </c>
+      <c r="O54" s="87">
+        <v>0</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="O54" s="9"/>
-    </row>
-    <row r="55" spans="1:15">
+      <c r="S54" s="9"/>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="8"/>
       <c r="B55" s="83" t="s">
         <v>206</v>
@@ -3681,14 +4351,26 @@
       <c r="K55" s="9">
         <v>0</v>
       </c>
-      <c r="L55" s="2"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="20" t="s">
+      <c r="L55" s="89">
+        <v>0</v>
+      </c>
+      <c r="M55" s="89">
+        <v>0</v>
+      </c>
+      <c r="N55" s="87">
+        <v>0</v>
+      </c>
+      <c r="O55" s="87">
+        <v>0</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="O55" s="9"/>
-    </row>
-    <row r="56" spans="1:15">
+      <c r="S55" s="9"/>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="8"/>
       <c r="B56" s="83" t="s">
         <v>207</v>
@@ -3720,14 +4402,26 @@
       <c r="K56" s="9">
         <v>0</v>
       </c>
-      <c r="L56" s="2"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="20" t="s">
+      <c r="L56" s="89">
+        <v>0</v>
+      </c>
+      <c r="M56" s="89">
+        <v>0</v>
+      </c>
+      <c r="N56" s="87">
+        <v>0</v>
+      </c>
+      <c r="O56" s="87">
+        <v>0</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="O56" s="9"/>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="S56" s="9"/>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="8"/>
       <c r="B57" s="83" t="s">
         <v>208</v>
@@ -3759,14 +4453,26 @@
       <c r="K57" s="9">
         <v>0</v>
       </c>
-      <c r="L57" s="2"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="20" t="s">
+      <c r="L57" s="89">
+        <v>0</v>
+      </c>
+      <c r="M57" s="89">
+        <v>0</v>
+      </c>
+      <c r="N57" s="87">
+        <v>0</v>
+      </c>
+      <c r="O57" s="87">
+        <v>0</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O57" s="9"/>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="S57" s="9"/>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" s="8"/>
       <c r="B58" s="83" t="s">
         <v>209</v>
@@ -3798,14 +4504,26 @@
       <c r="K58" s="9">
         <v>0</v>
       </c>
-      <c r="L58" s="2"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="20" t="s">
+      <c r="L58" s="89">
+        <v>0</v>
+      </c>
+      <c r="M58" s="89">
+        <v>0</v>
+      </c>
+      <c r="N58" s="87">
+        <v>0</v>
+      </c>
+      <c r="O58" s="87">
+        <v>0</v>
+      </c>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="O58" s="9"/>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="S58" s="9"/>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" s="8"/>
       <c r="B59" s="83" t="s">
         <v>210</v>
@@ -3837,14 +4555,26 @@
       <c r="K59" s="9">
         <v>0</v>
       </c>
-      <c r="L59" s="2"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="20" t="s">
+      <c r="L59" s="89">
+        <v>0</v>
+      </c>
+      <c r="M59" s="89">
+        <v>0</v>
+      </c>
+      <c r="N59" s="87">
+        <v>0</v>
+      </c>
+      <c r="O59" s="87">
+        <v>0</v>
+      </c>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="O59" s="9"/>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="S59" s="9"/>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" s="8"/>
       <c r="B60" s="83" t="s">
         <v>211</v>
@@ -3876,14 +4606,26 @@
       <c r="K60" s="9">
         <v>0</v>
       </c>
-      <c r="L60" s="2"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="20" t="s">
+      <c r="L60" s="89">
+        <v>0</v>
+      </c>
+      <c r="M60" s="89">
+        <v>0</v>
+      </c>
+      <c r="N60" s="87">
+        <v>0</v>
+      </c>
+      <c r="O60" s="87">
+        <v>0</v>
+      </c>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="O60" s="9"/>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="S60" s="9"/>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" s="8"/>
       <c r="B61" s="83" t="s">
         <v>212</v>
@@ -3915,14 +4657,26 @@
       <c r="K61" s="9">
         <v>0</v>
       </c>
-      <c r="L61" s="2"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="20" t="s">
+      <c r="L61" s="89">
+        <v>0</v>
+      </c>
+      <c r="M61" s="89">
+        <v>0</v>
+      </c>
+      <c r="N61" s="87">
+        <v>0</v>
+      </c>
+      <c r="O61" s="87">
+        <v>0</v>
+      </c>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="8"/>
+      <c r="R61" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="O61" s="9"/>
-    </row>
-    <row r="62" spans="1:15">
+      <c r="S61" s="9"/>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" s="8"/>
       <c r="B62" s="83" t="s">
         <v>213</v>
@@ -3954,14 +4708,26 @@
       <c r="K62" s="9">
         <v>0</v>
       </c>
-      <c r="L62" s="2"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="20" t="s">
+      <c r="L62" s="89">
+        <v>0</v>
+      </c>
+      <c r="M62" s="89">
+        <v>0</v>
+      </c>
+      <c r="N62" s="87">
+        <v>0</v>
+      </c>
+      <c r="O62" s="87">
+        <v>0</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="8"/>
+      <c r="R62" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="O62" s="9"/>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="S62" s="9"/>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" s="8"/>
       <c r="B63" s="83" t="s">
         <v>214</v>
@@ -3993,14 +4759,26 @@
       <c r="K63" s="9">
         <v>0</v>
       </c>
-      <c r="L63" s="2"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="20" t="s">
+      <c r="L63" s="89">
+        <v>0</v>
+      </c>
+      <c r="M63" s="89">
+        <v>0</v>
+      </c>
+      <c r="N63" s="87">
+        <v>0</v>
+      </c>
+      <c r="O63" s="87">
+        <v>0</v>
+      </c>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="O63" s="9"/>
-    </row>
-    <row r="64" spans="1:15">
+      <c r="S63" s="9"/>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" s="8"/>
       <c r="B64" s="83" t="s">
         <v>215</v>
@@ -4032,12 +4810,24 @@
       <c r="K64" s="9">
         <v>0</v>
       </c>
-      <c r="L64" s="2"/>
-      <c r="M64" s="8"/>
-      <c r="N64" s="20" t="s">
+      <c r="L64" s="89">
+        <v>0</v>
+      </c>
+      <c r="M64" s="89">
+        <v>0</v>
+      </c>
+      <c r="N64" s="87">
+        <v>0</v>
+      </c>
+      <c r="O64" s="87">
+        <v>0</v>
+      </c>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="8"/>
+      <c r="R64" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="O64" s="9"/>
+      <c r="S64" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4046,20 +4836,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="20.85546875" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="19"/>
+    <col min="10" max="13" width="25.5703125" style="58" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="33" customFormat="1" ht="81" customHeight="1">
+    <row r="1" spans="1:13" s="33" customFormat="1" ht="81" customHeight="1">
       <c r="A1" s="84" t="s">
         <v>1</v>
       </c>
@@ -4087,8 +4878,20 @@
       <c r="I1" s="32" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="30" customFormat="1">
+      <c r="J1" s="90" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" s="90" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="90" t="s">
+        <v>220</v>
+      </c>
+      <c r="M1" s="90" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="30" customFormat="1">
       <c r="A2" s="85" t="s">
         <v>2</v>
       </c>
@@ -4104,8 +4907,20 @@
         <v>90</v>
       </c>
       <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:9" s="30" customFormat="1">
+      <c r="J2" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="L2" s="86" t="s">
+        <v>222</v>
+      </c>
+      <c r="M2" s="86" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="30" customFormat="1">
       <c r="A3" s="85" t="s">
         <v>3</v>
       </c>
@@ -4133,8 +4948,20 @@
       <c r="I3" s="28" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="30" customFormat="1">
+      <c r="J3" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="30" customFormat="1">
       <c r="A4" s="85" t="s">
         <v>82</v>
       </c>
@@ -4150,8 +4977,12 @@
       </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="83" t="s">
         <v>160</v>
       </c>
@@ -4177,8 +5008,20 @@
       <c r="I5" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="89">
+        <v>40.453667103041987</v>
+      </c>
+      <c r="K5" s="89">
+        <v>3.8551462933222229</v>
+      </c>
+      <c r="L5" s="87">
+        <v>26.942537613293517</v>
+      </c>
+      <c r="M5" s="87">
+        <v>28.748648990342275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="83" t="s">
         <v>161</v>
       </c>
@@ -4204,8 +5047,20 @@
       <c r="I6" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="89">
+        <v>24.20655340611955</v>
+      </c>
+      <c r="K6" s="89">
+        <v>4.2099176569894787</v>
+      </c>
+      <c r="L6" s="87">
+        <v>33.503697246598598</v>
+      </c>
+      <c r="M6" s="87">
+        <v>38.079831690292373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="83" t="s">
         <v>162</v>
       </c>
@@ -4231,8 +5086,20 @@
       <c r="I7" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="89">
+        <v>37.922310101343321</v>
+      </c>
+      <c r="K7" s="89">
+        <v>16.894724535937865</v>
+      </c>
+      <c r="L7" s="87">
+        <v>38.969241119370921</v>
+      </c>
+      <c r="M7" s="87">
+        <v>6.2137242433478974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="83" t="s">
         <v>163</v>
       </c>
@@ -4258,8 +5125,20 @@
       <c r="I8" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="89">
+        <v>44.563130721438888</v>
+      </c>
+      <c r="K8" s="89">
+        <v>3.9864523347987388</v>
+      </c>
+      <c r="L8" s="87">
+        <v>25.613545462343208</v>
+      </c>
+      <c r="M8" s="87">
+        <v>25.836871481419166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="83" t="s">
         <v>164</v>
       </c>
@@ -4285,8 +5164,20 @@
       <c r="I9" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="89">
+        <v>44.563130721438853</v>
+      </c>
+      <c r="K9" s="89">
+        <v>3.9864523347987366</v>
+      </c>
+      <c r="L9" s="87">
+        <v>25.613545462343168</v>
+      </c>
+      <c r="M9" s="87">
+        <v>25.836871481419251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="83" t="s">
         <v>9</v>
       </c>
@@ -4312,8 +5203,20 @@
       <c r="I10" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="89">
+        <v>51.156662692132173</v>
+      </c>
+      <c r="K10" s="89">
+        <v>7.8841320437625262</v>
+      </c>
+      <c r="L10" s="87">
+        <v>26.799770977154484</v>
+      </c>
+      <c r="M10" s="87">
+        <v>14.159434286950813</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="83" t="s">
         <v>165</v>
       </c>
@@ -4339,8 +5242,20 @@
       <c r="I11" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="89">
+        <v>51.156662692132194</v>
+      </c>
+      <c r="K11" s="89">
+        <v>7.8841320437625289</v>
+      </c>
+      <c r="L11" s="87">
+        <v>26.799770977154502</v>
+      </c>
+      <c r="M11" s="87">
+        <v>14.159434286950784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="83" t="s">
         <v>11</v>
       </c>
@@ -4366,8 +5281,20 @@
       <c r="I12" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="89">
+        <v>44.027727796234672</v>
+      </c>
+      <c r="K12" s="89">
+        <v>13.453599157505661</v>
+      </c>
+      <c r="L12" s="87">
+        <v>33.979895620423065</v>
+      </c>
+      <c r="M12" s="87">
+        <v>8.5387774258365994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="83" t="s">
         <v>166</v>
       </c>
@@ -4393,8 +5320,20 @@
       <c r="I13" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="89">
+        <v>0</v>
+      </c>
+      <c r="K13" s="89">
+        <v>0</v>
+      </c>
+      <c r="L13" s="87">
+        <v>0</v>
+      </c>
+      <c r="M13" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="83" t="s">
         <v>13</v>
       </c>
@@ -4420,8 +5359,20 @@
       <c r="I14" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="89">
+        <v>45.254686949269271</v>
+      </c>
+      <c r="K14" s="89">
+        <v>12.692129498156582</v>
+      </c>
+      <c r="L14" s="87">
+        <v>32.917259248276224</v>
+      </c>
+      <c r="M14" s="87">
+        <v>9.1359243042979301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="83" t="s">
         <v>167</v>
       </c>
@@ -4447,8 +5398,20 @@
       <c r="I15" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="89">
+        <v>40.060402076129378</v>
+      </c>
+      <c r="K15" s="89">
+        <v>15.740031149967967</v>
+      </c>
+      <c r="L15" s="87">
+        <v>37.264467670202784</v>
+      </c>
+      <c r="M15" s="87">
+        <v>6.9350991036998693</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="83" t="s">
         <v>168</v>
       </c>
@@ -4474,8 +5437,20 @@
       <c r="I16" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="89">
+        <v>44.027727796234686</v>
+      </c>
+      <c r="K16" s="89">
+        <v>13.453599157505661</v>
+      </c>
+      <c r="L16" s="87">
+        <v>33.979895620423065</v>
+      </c>
+      <c r="M16" s="87">
+        <v>8.5387774258365852</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="83" t="s">
         <v>217</v>
       </c>
@@ -4501,8 +5476,20 @@
       <c r="I17" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="89">
+        <v>47.8240101290599</v>
+      </c>
+      <c r="K17" s="89">
+        <v>4.3160275423909011</v>
+      </c>
+      <c r="L17" s="87">
+        <v>24.785614004914009</v>
+      </c>
+      <c r="M17" s="87">
+        <v>23.074348323635192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="83" t="s">
         <v>169</v>
       </c>
@@ -4528,8 +5515,20 @@
       <c r="I18" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="89">
+        <v>47.824010129059872</v>
+      </c>
+      <c r="K18" s="89">
+        <v>4.3160275423908985</v>
+      </c>
+      <c r="L18" s="87">
+        <v>24.785614004914009</v>
+      </c>
+      <c r="M18" s="87">
+        <v>23.07434832363522</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="83" t="s">
         <v>170</v>
       </c>
@@ -4555,8 +5554,20 @@
       <c r="I19" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="89">
+        <v>40.060402076129392</v>
+      </c>
+      <c r="K19" s="89">
+        <v>15.740031149967976</v>
+      </c>
+      <c r="L19" s="87">
+        <v>37.264467670202784</v>
+      </c>
+      <c r="M19" s="87">
+        <v>6.935099103699855</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="83" t="s">
         <v>171</v>
       </c>
@@ -4582,8 +5593,20 @@
       <c r="I20" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="89">
+        <v>40.060402076129371</v>
+      </c>
+      <c r="K20" s="89">
+        <v>15.740031149967971</v>
+      </c>
+      <c r="L20" s="87">
+        <v>37.264467670202784</v>
+      </c>
+      <c r="M20" s="87">
+        <v>6.9350991036998835</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="83" t="s">
         <v>172</v>
       </c>
@@ -4609,8 +5632,20 @@
       <c r="I21" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="89">
+        <v>44.671577518796205</v>
+      </c>
+      <c r="K21" s="89">
+        <v>13.058173881020064</v>
+      </c>
+      <c r="L21" s="87">
+        <v>33.425889852467733</v>
+      </c>
+      <c r="M21" s="87">
+        <v>8.8443587477160008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="83" t="s">
         <v>173</v>
       </c>
@@ -4636,8 +5671,20 @@
       <c r="I22" s="25">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="89">
+        <v>47.82401012905985</v>
+      </c>
+      <c r="K22" s="89">
+        <v>4.3160275423909003</v>
+      </c>
+      <c r="L22" s="87">
+        <v>24.785614004913992</v>
+      </c>
+      <c r="M22" s="87">
+        <v>23.074348323635263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="83" t="s">
         <v>174</v>
       </c>
@@ -4663,8 +5710,20 @@
       <c r="I23" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="89">
+        <v>0</v>
+      </c>
+      <c r="K23" s="89">
+        <v>0</v>
+      </c>
+      <c r="L23" s="87">
+        <v>0</v>
+      </c>
+      <c r="M23" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="83" t="s">
         <v>175</v>
       </c>
@@ -4690,8 +5749,20 @@
       <c r="I24" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="89">
+        <v>0</v>
+      </c>
+      <c r="K24" s="89">
+        <v>0</v>
+      </c>
+      <c r="L24" s="87">
+        <v>0</v>
+      </c>
+      <c r="M24" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="83" t="s">
         <v>176</v>
       </c>
@@ -4717,8 +5788,20 @@
       <c r="I25" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="89">
+        <v>0</v>
+      </c>
+      <c r="K25" s="89">
+        <v>0</v>
+      </c>
+      <c r="L25" s="87">
+        <v>0</v>
+      </c>
+      <c r="M25" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="83" t="s">
         <v>177</v>
       </c>
@@ -4744,8 +5827,20 @@
       <c r="I26" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="89">
+        <v>0</v>
+      </c>
+      <c r="K26" s="89">
+        <v>0</v>
+      </c>
+      <c r="L26" s="87">
+        <v>0</v>
+      </c>
+      <c r="M26" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="83" t="s">
         <v>178</v>
       </c>
@@ -4771,8 +5866,20 @@
       <c r="I27" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="89">
+        <v>0</v>
+      </c>
+      <c r="K27" s="89">
+        <v>0</v>
+      </c>
+      <c r="L27" s="87">
+        <v>0</v>
+      </c>
+      <c r="M27" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="83" t="s">
         <v>179</v>
       </c>
@@ -4798,8 +5905,20 @@
       <c r="I28" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="89">
+        <v>0</v>
+      </c>
+      <c r="K28" s="89">
+        <v>0</v>
+      </c>
+      <c r="L28" s="87">
+        <v>0</v>
+      </c>
+      <c r="M28" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="83" t="s">
         <v>180</v>
       </c>
@@ -4825,8 +5944,20 @@
       <c r="I29" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="89">
+        <v>0</v>
+      </c>
+      <c r="K29" s="89">
+        <v>0</v>
+      </c>
+      <c r="L29" s="87">
+        <v>0</v>
+      </c>
+      <c r="M29" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="83" t="s">
         <v>181</v>
       </c>
@@ -4852,8 +5983,20 @@
       <c r="I30" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="89">
+        <v>0</v>
+      </c>
+      <c r="K30" s="89">
+        <v>0</v>
+      </c>
+      <c r="L30" s="87">
+        <v>0</v>
+      </c>
+      <c r="M30" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="83" t="s">
         <v>182</v>
       </c>
@@ -4879,8 +6022,20 @@
       <c r="I31" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="89">
+        <v>0</v>
+      </c>
+      <c r="K31" s="89">
+        <v>0</v>
+      </c>
+      <c r="L31" s="87">
+        <v>0</v>
+      </c>
+      <c r="M31" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="83" t="s">
         <v>183</v>
       </c>
@@ -4906,8 +6061,20 @@
       <c r="I32" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="89">
+        <v>0</v>
+      </c>
+      <c r="K32" s="89">
+        <v>0</v>
+      </c>
+      <c r="L32" s="87">
+        <v>0</v>
+      </c>
+      <c r="M32" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="83" t="s">
         <v>184</v>
       </c>
@@ -4933,8 +6100,20 @@
       <c r="I33" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="89">
+        <v>0</v>
+      </c>
+      <c r="K33" s="89">
+        <v>0</v>
+      </c>
+      <c r="L33" s="87">
+        <v>0</v>
+      </c>
+      <c r="M33" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="83" t="s">
         <v>185</v>
       </c>
@@ -4960,8 +6139,20 @@
       <c r="I34" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="89">
+        <v>0</v>
+      </c>
+      <c r="K34" s="89">
+        <v>0</v>
+      </c>
+      <c r="L34" s="87">
+        <v>0</v>
+      </c>
+      <c r="M34" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="83" t="s">
         <v>186</v>
       </c>
@@ -4987,8 +6178,20 @@
       <c r="I35" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" s="89">
+        <v>0</v>
+      </c>
+      <c r="K35" s="89">
+        <v>0</v>
+      </c>
+      <c r="L35" s="87">
+        <v>0</v>
+      </c>
+      <c r="M35" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="83" t="s">
         <v>187</v>
       </c>
@@ -5014,8 +6217,20 @@
       <c r="I36" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" s="89">
+        <v>0</v>
+      </c>
+      <c r="K36" s="89">
+        <v>0</v>
+      </c>
+      <c r="L36" s="87">
+        <v>0</v>
+      </c>
+      <c r="M36" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="83" t="s">
         <v>188</v>
       </c>
@@ -5041,8 +6256,20 @@
       <c r="I37" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" s="89">
+        <v>0</v>
+      </c>
+      <c r="K37" s="89">
+        <v>0</v>
+      </c>
+      <c r="L37" s="87">
+        <v>0</v>
+      </c>
+      <c r="M37" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="83" t="s">
         <v>189</v>
       </c>
@@ -5068,8 +6295,20 @@
       <c r="I38" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" s="89">
+        <v>0</v>
+      </c>
+      <c r="K38" s="89">
+        <v>0</v>
+      </c>
+      <c r="L38" s="87">
+        <v>0</v>
+      </c>
+      <c r="M38" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="83" t="s">
         <v>190</v>
       </c>
@@ -5095,8 +6334,20 @@
       <c r="I39" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" s="89">
+        <v>0</v>
+      </c>
+      <c r="K39" s="89">
+        <v>0</v>
+      </c>
+      <c r="L39" s="87">
+        <v>0</v>
+      </c>
+      <c r="M39" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="83" t="s">
         <v>191</v>
       </c>
@@ -5122,8 +6373,20 @@
       <c r="I40" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" s="89">
+        <v>0</v>
+      </c>
+      <c r="K40" s="89">
+        <v>0</v>
+      </c>
+      <c r="L40" s="87">
+        <v>0</v>
+      </c>
+      <c r="M40" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="83" t="s">
         <v>192</v>
       </c>
@@ -5149,8 +6412,20 @@
       <c r="I41" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" s="89">
+        <v>0</v>
+      </c>
+      <c r="K41" s="89">
+        <v>0</v>
+      </c>
+      <c r="L41" s="87">
+        <v>0</v>
+      </c>
+      <c r="M41" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="83" t="s">
         <v>193</v>
       </c>
@@ -5176,8 +6451,20 @@
       <c r="I42" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" s="89">
+        <v>0</v>
+      </c>
+      <c r="K42" s="89">
+        <v>0</v>
+      </c>
+      <c r="L42" s="87">
+        <v>0</v>
+      </c>
+      <c r="M42" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="83" t="s">
         <v>194</v>
       </c>
@@ -5203,8 +6490,20 @@
       <c r="I43" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" s="89">
+        <v>51.265859991640617</v>
+      </c>
+      <c r="K43" s="89">
+        <v>5.5695962486522026</v>
+      </c>
+      <c r="L43" s="87">
+        <v>24.73507248608006</v>
+      </c>
+      <c r="M43" s="87">
+        <v>18.429471273627115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="83" t="s">
         <v>195</v>
       </c>
@@ -5230,8 +6529,20 @@
       <c r="I44" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" s="89">
+        <v>0</v>
+      </c>
+      <c r="K44" s="89">
+        <v>0</v>
+      </c>
+      <c r="L44" s="87">
+        <v>0</v>
+      </c>
+      <c r="M44" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="83" t="s">
         <v>196</v>
       </c>
@@ -5257,8 +6568,20 @@
       <c r="I45" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" s="89">
+        <v>0</v>
+      </c>
+      <c r="K45" s="89">
+        <v>0</v>
+      </c>
+      <c r="L45" s="87">
+        <v>0</v>
+      </c>
+      <c r="M45" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="83" t="s">
         <v>197</v>
       </c>
@@ -5284,8 +6607,20 @@
       <c r="I46" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" s="89">
+        <v>0</v>
+      </c>
+      <c r="K46" s="89">
+        <v>0</v>
+      </c>
+      <c r="L46" s="87">
+        <v>0</v>
+      </c>
+      <c r="M46" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="83" t="s">
         <v>198</v>
       </c>
@@ -5311,8 +6646,20 @@
       <c r="I47" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" s="89">
+        <v>0</v>
+      </c>
+      <c r="K47" s="89">
+        <v>0</v>
+      </c>
+      <c r="L47" s="87">
+        <v>0</v>
+      </c>
+      <c r="M47" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="83" t="s">
         <v>199</v>
       </c>
@@ -5338,8 +6685,20 @@
       <c r="I48" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" s="89">
+        <v>0</v>
+      </c>
+      <c r="K48" s="89">
+        <v>0</v>
+      </c>
+      <c r="L48" s="87">
+        <v>0</v>
+      </c>
+      <c r="M48" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="83" t="s">
         <v>200</v>
       </c>
@@ -5365,8 +6724,20 @@
       <c r="I49" s="25">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" s="89">
+        <v>0</v>
+      </c>
+      <c r="K49" s="89">
+        <v>0</v>
+      </c>
+      <c r="L49" s="87">
+        <v>0</v>
+      </c>
+      <c r="M49" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="83" t="s">
         <v>201</v>
       </c>
@@ -5382,8 +6753,20 @@
         <v>0</v>
       </c>
       <c r="I50" s="25"/>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" s="89">
+        <v>44.027727796234686</v>
+      </c>
+      <c r="K50" s="89">
+        <v>13.453599157505671</v>
+      </c>
+      <c r="L50" s="87">
+        <v>33.979895620423086</v>
+      </c>
+      <c r="M50" s="87">
+        <v>8.5387774258365567</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="83" t="s">
         <v>202</v>
       </c>
@@ -5399,8 +6782,20 @@
         <v>0</v>
       </c>
       <c r="I51" s="25"/>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" s="89">
+        <v>0</v>
+      </c>
+      <c r="K51" s="89">
+        <v>0</v>
+      </c>
+      <c r="L51" s="87">
+        <v>0</v>
+      </c>
+      <c r="M51" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="83" t="s">
         <v>203</v>
       </c>
@@ -5416,8 +6811,20 @@
         <v>0</v>
       </c>
       <c r="I52" s="25"/>
-    </row>
-    <row r="53" spans="1:9">
+      <c r="J52" s="89">
+        <v>0</v>
+      </c>
+      <c r="K52" s="89">
+        <v>0</v>
+      </c>
+      <c r="L52" s="87">
+        <v>0</v>
+      </c>
+      <c r="M52" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" s="83" t="s">
         <v>204</v>
       </c>
@@ -5433,8 +6840,20 @@
         <v>0</v>
       </c>
       <c r="I53" s="25"/>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" s="89">
+        <v>0</v>
+      </c>
+      <c r="K53" s="89">
+        <v>0</v>
+      </c>
+      <c r="L53" s="87">
+        <v>0</v>
+      </c>
+      <c r="M53" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="83" t="s">
         <v>205</v>
       </c>
@@ -5450,8 +6869,20 @@
         <v>0</v>
       </c>
       <c r="I54" s="25"/>
-    </row>
-    <row r="55" spans="1:9">
+      <c r="J54" s="89">
+        <v>0</v>
+      </c>
+      <c r="K54" s="89">
+        <v>0</v>
+      </c>
+      <c r="L54" s="87">
+        <v>0</v>
+      </c>
+      <c r="M54" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="83" t="s">
         <v>206</v>
       </c>
@@ -5467,8 +6898,20 @@
         <v>0</v>
       </c>
       <c r="I55" s="25"/>
-    </row>
-    <row r="56" spans="1:9">
+      <c r="J55" s="89">
+        <v>0</v>
+      </c>
+      <c r="K55" s="89">
+        <v>0</v>
+      </c>
+      <c r="L55" s="87">
+        <v>0</v>
+      </c>
+      <c r="M55" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="83" t="s">
         <v>207</v>
       </c>
@@ -5484,8 +6927,20 @@
         <v>0</v>
       </c>
       <c r="I56" s="25"/>
-    </row>
-    <row r="57" spans="1:9">
+      <c r="J56" s="89">
+        <v>0</v>
+      </c>
+      <c r="K56" s="89">
+        <v>0</v>
+      </c>
+      <c r="L56" s="87">
+        <v>0</v>
+      </c>
+      <c r="M56" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="83" t="s">
         <v>208</v>
       </c>
@@ -5501,8 +6956,20 @@
         <v>0</v>
       </c>
       <c r="I57" s="25"/>
-    </row>
-    <row r="58" spans="1:9">
+      <c r="J57" s="89">
+        <v>0</v>
+      </c>
+      <c r="K57" s="89">
+        <v>0</v>
+      </c>
+      <c r="L57" s="87">
+        <v>0</v>
+      </c>
+      <c r="M57" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="83" t="s">
         <v>209</v>
       </c>
@@ -5518,8 +6985,20 @@
         <v>0</v>
       </c>
       <c r="I58" s="25"/>
-    </row>
-    <row r="59" spans="1:9">
+      <c r="J58" s="89">
+        <v>0</v>
+      </c>
+      <c r="K58" s="89">
+        <v>0</v>
+      </c>
+      <c r="L58" s="87">
+        <v>0</v>
+      </c>
+      <c r="M58" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="83" t="s">
         <v>210</v>
       </c>
@@ -5535,8 +7014,20 @@
         <v>0</v>
       </c>
       <c r="I59" s="25"/>
-    </row>
-    <row r="60" spans="1:9">
+      <c r="J59" s="89">
+        <v>0</v>
+      </c>
+      <c r="K59" s="89">
+        <v>0</v>
+      </c>
+      <c r="L59" s="87">
+        <v>0</v>
+      </c>
+      <c r="M59" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="83" t="s">
         <v>211</v>
       </c>
@@ -5552,8 +7043,20 @@
         <v>0</v>
       </c>
       <c r="I60" s="25"/>
-    </row>
-    <row r="61" spans="1:9">
+      <c r="J60" s="89">
+        <v>0</v>
+      </c>
+      <c r="K60" s="89">
+        <v>0</v>
+      </c>
+      <c r="L60" s="87">
+        <v>0</v>
+      </c>
+      <c r="M60" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="83" t="s">
         <v>212</v>
       </c>
@@ -5569,8 +7072,20 @@
         <v>0</v>
       </c>
       <c r="I61" s="25"/>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" s="89">
+        <v>0</v>
+      </c>
+      <c r="K61" s="89">
+        <v>0</v>
+      </c>
+      <c r="L61" s="87">
+        <v>0</v>
+      </c>
+      <c r="M61" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="83" t="s">
         <v>213</v>
       </c>
@@ -5586,8 +7101,20 @@
         <v>0</v>
       </c>
       <c r="I62" s="25"/>
-    </row>
-    <row r="63" spans="1:9">
+      <c r="J62" s="89">
+        <v>0</v>
+      </c>
+      <c r="K62" s="89">
+        <v>0</v>
+      </c>
+      <c r="L62" s="87">
+        <v>0</v>
+      </c>
+      <c r="M62" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="83" t="s">
         <v>214</v>
       </c>
@@ -5603,8 +7130,20 @@
         <v>0</v>
       </c>
       <c r="I63" s="25"/>
-    </row>
-    <row r="64" spans="1:9">
+      <c r="J63" s="89">
+        <v>0</v>
+      </c>
+      <c r="K63" s="89">
+        <v>0</v>
+      </c>
+      <c r="L63" s="87">
+        <v>0</v>
+      </c>
+      <c r="M63" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="83" t="s">
         <v>215</v>
       </c>
@@ -5620,6 +7159,18 @@
         <v>0</v>
       </c>
       <c r="I64" s="25"/>
+      <c r="J64" s="89">
+        <v>0</v>
+      </c>
+      <c r="K64" s="89">
+        <v>0</v>
+      </c>
+      <c r="L64" s="87">
+        <v>0</v>
+      </c>
+      <c r="M64" s="87">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="6:9">
       <c r="F65" s="24"/>
@@ -13901,8 +15452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B64"/>
+    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
adding uncertainty from inputs to MC class
</commit_message>
<xml_diff>
--- a/Material properties - process modles.xlsx
+++ b/Material properties - process modles.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msmsa\Google Drive\Brightway2\Laptop_BitBucket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro H\Documents\NCSU\LCA\test-gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8840BE59-74D6-4C45-9F6B-C06434350F48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Composting" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="MW.MRF" sheetId="6" r:id="rId6"/>
     <sheet name="DS.MRF" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -891,7 +890,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -1430,57 +1429,57 @@
     </xf>
   </cellXfs>
   <cellStyles count="51">
-    <cellStyle name="Currency 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Currency 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Hyperlink 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="27" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Currency 2" xfId="40"/>
+    <cellStyle name="Currency 3" xfId="26"/>
+    <cellStyle name="Hyperlink 2" xfId="32"/>
+    <cellStyle name="Hyperlink 3" xfId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 2 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 2 2 3" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 2 2 4" xfId="14" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 2 2 5" xfId="17" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 2 2 6" xfId="20" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 2 2 7" xfId="23" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 2 2 8" xfId="8" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal 2 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal 2 3 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normal 2 4" xfId="10" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Normal 2 4 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Normal 2 5" xfId="16" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Normal 2 5 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Normal 2 6" xfId="19" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Normal 2 6 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 2 7" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 2 7 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 3" xfId="18" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 3 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 3 3" xfId="38" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 4" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 4 2" xfId="39" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 6" xfId="15" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 6 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 7" xfId="21" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 8" xfId="2" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 8 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 8 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 8 3" xfId="28" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 8 4" xfId="47" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 9" xfId="30" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 9 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Normal 9 3" xfId="48" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Normal_changes" xfId="3" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal_MRF" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Percent 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Percent 3" xfId="25" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Percent 3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Percent 3 3" xfId="29" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Percent 3 4" xfId="49" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 2 2" xfId="6"/>
+    <cellStyle name="Normal 2 2 2" xfId="9"/>
+    <cellStyle name="Normal 2 2 3" xfId="12"/>
+    <cellStyle name="Normal 2 2 4" xfId="14"/>
+    <cellStyle name="Normal 2 2 5" xfId="17"/>
+    <cellStyle name="Normal 2 2 6" xfId="20"/>
+    <cellStyle name="Normal 2 2 7" xfId="23"/>
+    <cellStyle name="Normal 2 2 8" xfId="8"/>
+    <cellStyle name="Normal 2 3" xfId="11"/>
+    <cellStyle name="Normal 2 3 2" xfId="33"/>
+    <cellStyle name="Normal 2 4" xfId="10"/>
+    <cellStyle name="Normal 2 4 2" xfId="34"/>
+    <cellStyle name="Normal 2 5" xfId="16"/>
+    <cellStyle name="Normal 2 5 2" xfId="35"/>
+    <cellStyle name="Normal 2 6" xfId="19"/>
+    <cellStyle name="Normal 2 6 2" xfId="36"/>
+    <cellStyle name="Normal 2 7" xfId="22"/>
+    <cellStyle name="Normal 2 7 2" xfId="37"/>
+    <cellStyle name="Normal 3" xfId="18"/>
+    <cellStyle name="Normal 3 2" xfId="31"/>
+    <cellStyle name="Normal 3 2 2" xfId="44"/>
+    <cellStyle name="Normal 3 3" xfId="38"/>
+    <cellStyle name="Normal 4" xfId="24"/>
+    <cellStyle name="Normal 4 2" xfId="39"/>
+    <cellStyle name="Normal 5" xfId="13"/>
+    <cellStyle name="Normal 6" xfId="15"/>
+    <cellStyle name="Normal 6 2" xfId="46"/>
+    <cellStyle name="Normal 7" xfId="21"/>
+    <cellStyle name="Normal 8" xfId="2"/>
+    <cellStyle name="Normal 8 2" xfId="41"/>
+    <cellStyle name="Normal 8 2 2" xfId="50"/>
+    <cellStyle name="Normal 8 3" xfId="28"/>
+    <cellStyle name="Normal 8 4" xfId="47"/>
+    <cellStyle name="Normal 9" xfId="30"/>
+    <cellStyle name="Normal 9 2" xfId="43"/>
+    <cellStyle name="Normal 9 3" xfId="48"/>
+    <cellStyle name="Normal_changes" xfId="3"/>
+    <cellStyle name="Normal_MRF" xfId="45"/>
+    <cellStyle name="Percent 2" xfId="4"/>
+    <cellStyle name="Percent 2 2" xfId="7"/>
+    <cellStyle name="Percent 3" xfId="25"/>
+    <cellStyle name="Percent 3 2" xfId="42"/>
+    <cellStyle name="Percent 3 3" xfId="29"/>
+    <cellStyle name="Percent 3 4" xfId="49"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1757,25 +1756,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O1" sqref="L1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7265625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="25.54296875" style="19" customWidth="1"/>
-    <col min="12" max="15" width="25.54296875" style="56" customWidth="1"/>
-    <col min="16" max="17" width="25.54296875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="25.5703125" style="19" customWidth="1"/>
+    <col min="12" max="15" width="25.5703125" style="56" customWidth="1"/>
+    <col min="16" max="17" width="25.5703125" style="19" customWidth="1"/>
     <col min="18" max="18" width="31" style="22" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="24" style="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="67" width="25.54296875" style="19" customWidth="1"/>
-    <col min="68" max="16384" width="9.1796875" style="19"/>
+    <col min="20" max="67" width="25.5703125" style="19" customWidth="1"/>
+    <col min="68" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="16" customFormat="1" ht="81" customHeight="1">
@@ -5020,19 +5019,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="20.81640625" style="19" customWidth="1"/>
-    <col min="10" max="13" width="25.54296875" style="56" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="19"/>
+    <col min="2" max="9" width="20.85546875" style="19" customWidth="1"/>
+    <col min="10" max="13" width="25.5703125" style="56" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="33" customFormat="1" ht="81" customHeight="1">
@@ -7381,30 +7380,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.7265625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="52.453125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" style="56" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="35" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.7265625" style="35" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="35"/>
+    <col min="11" max="11" width="28.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="44" customFormat="1" ht="58">
+    <row r="1" spans="1:16" s="44" customFormat="1" ht="60">
       <c r="A1" s="41" t="s">
         <v>94</v>
       </c>
@@ -8701,68 +8700,68 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="AJ26" sqref="AE26:AJ39"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7265625" style="56" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="56" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.1796875" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.90625" style="56" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6328125" style="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.90625" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.1796875" style="56" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.1796875" style="56" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.08984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.36328125" style="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.42578125" style="56" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="56" customWidth="1"/>
     <col min="13" max="13" width="9" style="56" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="56"/>
+    <col min="14" max="14" width="9.140625" style="56"/>
     <col min="15" max="15" width="9" style="56" bestFit="1" customWidth="1"/>
-    <col min="16" max="22" width="9.1796875" style="56"/>
+    <col min="16" max="22" width="9.140625" style="56"/>
     <col min="23" max="23" width="22" style="56" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.08984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="8.6328125" style="56" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1796875" style="56"/>
-    <col min="29" max="29" width="8.6328125" style="56" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.7265625" style="56" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.08984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="8.81640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="9.1796875" style="56"/>
-    <col min="36" max="36" width="8.81640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="8.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="56"/>
+    <col min="29" max="29" width="8.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.7109375" style="56" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="8.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="9.140625" style="56"/>
+    <col min="36" max="36" width="8.85546875" style="56" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9" style="56" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10" style="56" bestFit="1" customWidth="1"/>
     <col min="39" max="41" width="9" style="56" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.1796875" style="56"/>
-    <col min="43" max="43" width="9.54296875" style="56" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.90625" style="56" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="9.08984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="9.1796875" style="56"/>
-    <col min="50" max="50" width="9.08984375" style="56" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.1796875" style="56"/>
+    <col min="42" max="42" width="9.140625" style="56"/>
+    <col min="43" max="43" width="9.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="9.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="9.140625" style="56"/>
+    <col min="50" max="50" width="9.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.140625" style="56"/>
     <col min="52" max="52" width="10" style="56" bestFit="1" customWidth="1"/>
     <col min="53" max="55" width="9" style="56" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.1796875" style="56"/>
-    <col min="57" max="57" width="9.54296875" style="56" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="56"/>
+    <col min="57" max="57" width="9.5703125" style="56" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="10" style="56" bestFit="1" customWidth="1"/>
-    <col min="59" max="64" width="9.1796875" style="56"/>
+    <col min="59" max="64" width="9.140625" style="56"/>
     <col min="65" max="65" width="9" style="56" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="10" style="56" bestFit="1" customWidth="1"/>
     <col min="67" max="69" width="9" style="56" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="9.1796875" style="56"/>
-    <col min="71" max="71" width="9.54296875" style="56" bestFit="1" customWidth="1"/>
-    <col min="72" max="16384" width="9.1796875" style="56"/>
+    <col min="70" max="70" width="9.140625" style="56"/>
+    <col min="71" max="71" width="9.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="72" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="16" customFormat="1" ht="130.5">
+    <row r="1" spans="1:71" s="16" customFormat="1" ht="150">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
@@ -9118,7 +9117,7 @@
       <c r="BR3" s="52"/>
       <c r="BS3" s="52"/>
     </row>
-    <row r="4" spans="1:71" ht="29">
+    <row r="4" spans="1:71" ht="45">
       <c r="A4" s="34" t="s">
         <v>82</v>
       </c>
@@ -10367,9 +10366,15 @@
       <c r="I17" s="53">
         <v>1.3360000000000001</v>
       </c>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
+      <c r="J17" s="53">
+        <v>3</v>
+      </c>
+      <c r="K17" s="53">
+        <v>1.3</v>
+      </c>
+      <c r="L17" s="53">
+        <v>0.3</v>
+      </c>
       <c r="M17" s="53"/>
       <c r="N17" s="53"/>
       <c r="O17" s="53"/>
@@ -10453,12 +10458,22 @@
       <c r="B18" s="39">
         <v>1</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="C18" s="89">
+        <v>3</v>
+      </c>
+      <c r="D18" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="E18" s="39">
+        <v>0.05</v>
+      </c>
       <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+      <c r="G18" s="39">
+        <v>0.8</v>
+      </c>
+      <c r="H18" s="39">
+        <v>1</v>
+      </c>
       <c r="I18" s="54">
         <v>1.3360000000000001</v>
       </c>
@@ -10738,18 +10753,34 @@
       <c r="B21" s="39">
         <v>1</v>
       </c>
-      <c r="C21" s="89"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
+      <c r="C21" s="89">
+        <v>3</v>
+      </c>
+      <c r="D21" s="39">
+        <v>0.9</v>
+      </c>
+      <c r="E21" s="39">
+        <v>0.05</v>
+      </c>
       <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
+      <c r="G21" s="39">
+        <v>0.8</v>
+      </c>
+      <c r="H21" s="39">
+        <v>1</v>
+      </c>
       <c r="I21" s="53">
         <v>1.3360000000000001</v>
       </c>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
+      <c r="J21" s="53">
+        <v>3</v>
+      </c>
+      <c r="K21" s="53">
+        <v>1.3</v>
+      </c>
+      <c r="L21" s="53">
+        <v>0.3</v>
+      </c>
       <c r="M21" s="53"/>
       <c r="N21" s="53"/>
       <c r="O21" s="53"/>
@@ -14886,21 +14917,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD64"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="59.54296875" style="74" customWidth="1"/>
-    <col min="2" max="2" width="48.453125" customWidth="1"/>
+    <col min="1" max="1" width="59.5703125" style="74" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
     <col min="3" max="30" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="64" customFormat="1" ht="58">
+    <row r="1" spans="1:30" s="64" customFormat="1" ht="60">
       <c r="A1" s="50" t="s">
         <v>94</v>
       </c>
@@ -17210,21 +17241,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" style="74" customWidth="1"/>
-    <col min="2" max="2" width="50.81640625" customWidth="1"/>
-    <col min="3" max="31" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" customWidth="1"/>
+    <col min="3" max="31" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="67" customFormat="1" ht="72.5">
+    <row r="1" spans="1:31" s="67" customFormat="1" ht="90">
       <c r="A1" s="40" t="s">
         <v>94</v>
       </c>
@@ -19618,21 +19649,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF70"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.1796875" style="74" customWidth="1"/>
-    <col min="2" max="2" width="49.26953125" customWidth="1"/>
-    <col min="3" max="31" width="16.26953125" customWidth="1"/>
+    <col min="1" max="1" width="65.140625" style="74" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="3" max="31" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="67" customFormat="1" ht="43.5">
+    <row r="1" spans="1:31" s="67" customFormat="1" ht="60">
       <c r="A1" s="40" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
SS_MRF Mass calculations Resource use calculations
</commit_message>
<xml_diff>
--- a/Material properties - process modles.xlsx
+++ b/Material properties - process modles.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msardar2\Google Drive\Brightway2\Laptop_BitBucket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msardar2\Google Drive\Brightway2\PySWOLF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Composting" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="MW_MRF" sheetId="6" r:id="rId6"/>
     <sheet name="DS_MRF" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="283">
   <si>
     <t>Substrate mass flows inputs</t>
   </si>
@@ -885,9 +885,6 @@
   </si>
   <si>
     <t>Fraction of Recoverable Cu Oxidized During Combustion Maximum</t>
-  </si>
-  <si>
-    <t>Drum Feeder</t>
   </si>
 </sst>
 </file>
@@ -14915,116 +14912,112 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD61"/>
+  <dimension ref="A1:AC61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48.42578125" style="87" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="87" customWidth="1"/>
-    <col min="3" max="30" width="17" customWidth="1"/>
+    <col min="2" max="29" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="62" customFormat="1" ht="30">
+    <row r="1" spans="1:29" s="62" customFormat="1" ht="30">
       <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>283</v>
+        <v>103</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="F1" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="G1" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="H1" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="I1" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="J1" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="K1" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="L1" s="48" t="s">
         <v>139</v>
       </c>
+      <c r="M1" s="47" t="s">
+        <v>140</v>
+      </c>
       <c r="N1" s="47" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O1" s="47" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P1" s="47" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="R1" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="S1" s="61" t="s">
+      <c r="R1" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="S1" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="T1" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="V1" s="47" t="s">
+      <c r="U1" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="V1" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="X1" s="47" t="s">
+      <c r="W1" s="47" t="s">
         <v>150</v>
       </c>
+      <c r="X1" s="61" t="s">
+        <v>151</v>
+      </c>
       <c r="Y1" s="61" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Z1" s="61" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA1" s="61" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AB1" s="61" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AC1" s="61" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD1" s="61" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:29">
       <c r="A2" s="86" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="73"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="58"/>
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
@@ -15052,13 +15045,12 @@
       <c r="AA2" s="58"/>
       <c r="AB2" s="58"/>
       <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
-    </row>
-    <row r="3" spans="1:30">
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="74"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
       <c r="E3" s="59"/>
@@ -15086,13 +15078,12 @@
       <c r="AA3" s="59"/>
       <c r="AB3" s="59"/>
       <c r="AC3" s="59"/>
-      <c r="AD3" s="59"/>
-    </row>
-    <row r="4" spans="1:30">
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="B4" s="75"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
       <c r="E4" s="60"/>
@@ -15120,13 +15111,12 @@
       <c r="AA4" s="60"/>
       <c r="AB4" s="60"/>
       <c r="AC4" s="60"/>
-      <c r="AD4" s="60"/>
-    </row>
-    <row r="5" spans="1:30">
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="86" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="59"/>
       <c r="D5" s="59"/>
       <c r="E5" s="59"/>
@@ -15154,13 +15144,12 @@
       <c r="AA5" s="59"/>
       <c r="AB5" s="59"/>
       <c r="AC5" s="59"/>
-      <c r="AD5" s="59"/>
-    </row>
-    <row r="6" spans="1:30">
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
       <c r="E6" s="60"/>
@@ -15188,13 +15177,12 @@
       <c r="AA6" s="60"/>
       <c r="AB6" s="60"/>
       <c r="AC6" s="60"/>
-      <c r="AD6" s="60"/>
-    </row>
-    <row r="7" spans="1:30">
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="74"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="59"/>
       <c r="D7" s="59"/>
       <c r="E7" s="59"/>
@@ -15222,13 +15210,12 @@
       <c r="AA7" s="59"/>
       <c r="AB7" s="59"/>
       <c r="AC7" s="59"/>
-      <c r="AD7" s="59"/>
-    </row>
-    <row r="8" spans="1:30">
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" s="86" t="s">
         <v>165</v>
       </c>
-      <c r="B8" s="75"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="60"/>
       <c r="D8" s="60"/>
       <c r="E8" s="60"/>
@@ -15256,13 +15243,12 @@
       <c r="AA8" s="60"/>
       <c r="AB8" s="60"/>
       <c r="AC8" s="60"/>
-      <c r="AD8" s="60"/>
-    </row>
-    <row r="9" spans="1:30">
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="74"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="59"/>
       <c r="D9" s="59"/>
       <c r="E9" s="59"/>
@@ -15290,13 +15276,12 @@
       <c r="AA9" s="59"/>
       <c r="AB9" s="59"/>
       <c r="AC9" s="59"/>
-      <c r="AD9" s="59"/>
-    </row>
-    <row r="10" spans="1:30">
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="B10" s="75"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="60"/>
       <c r="D10" s="60"/>
       <c r="E10" s="60"/>
@@ -15324,31 +15309,30 @@
       <c r="AA10" s="60"/>
       <c r="AB10" s="60"/>
       <c r="AC10" s="60"/>
-      <c r="AD10" s="60"/>
-    </row>
-    <row r="11" spans="1:30">
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="74"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="59"/>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
       <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
+      <c r="H11" s="59">
+        <v>0.88</v>
+      </c>
       <c r="I11" s="59">
+        <v>0</v>
+      </c>
+      <c r="J11" s="59">
         <v>0.88</v>
       </c>
-      <c r="J11" s="59">
-        <v>0</v>
-      </c>
       <c r="K11" s="59">
-        <v>0.88</v>
-      </c>
-      <c r="L11" s="59">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L11" s="59"/>
       <c r="M11" s="59"/>
       <c r="N11" s="59"/>
       <c r="O11" s="59"/>
@@ -15366,35 +15350,34 @@
       <c r="AA11" s="59"/>
       <c r="AB11" s="59"/>
       <c r="AC11" s="59"/>
-      <c r="AD11" s="59"/>
-    </row>
-    <row r="12" spans="1:30">
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12" s="86" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="75"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="60"/>
       <c r="D12" s="60"/>
       <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
+      <c r="F12" s="60">
+        <v>0</v>
+      </c>
       <c r="G12" s="60">
         <v>0</v>
       </c>
       <c r="H12" s="60">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="I12" s="60">
+        <v>0</v>
+      </c>
+      <c r="J12" s="60">
         <v>0.88</v>
       </c>
-      <c r="J12" s="60">
-        <v>0</v>
-      </c>
       <c r="K12" s="60">
-        <v>0.88</v>
-      </c>
-      <c r="L12" s="60">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L12" s="60"/>
       <c r="M12" s="60"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
@@ -15412,31 +15395,30 @@
       <c r="AA12" s="60"/>
       <c r="AB12" s="60"/>
       <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-    </row>
-    <row r="13" spans="1:30">
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13" s="86" t="s">
         <v>168</v>
       </c>
-      <c r="B13" s="74"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="59"/>
       <c r="D13" s="59"/>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
       <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
+      <c r="H13" s="59">
+        <v>0.88</v>
+      </c>
       <c r="I13" s="59">
+        <v>0</v>
+      </c>
+      <c r="J13" s="59">
         <v>0.88</v>
       </c>
-      <c r="J13" s="59">
-        <v>0</v>
-      </c>
       <c r="K13" s="59">
-        <v>0.88</v>
-      </c>
-      <c r="L13" s="59">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L13" s="59"/>
       <c r="M13" s="59"/>
       <c r="N13" s="59"/>
       <c r="O13" s="59"/>
@@ -15454,31 +15436,30 @@
       <c r="AA13" s="59"/>
       <c r="AB13" s="59"/>
       <c r="AC13" s="59"/>
-      <c r="AD13" s="59"/>
-    </row>
-    <row r="14" spans="1:30">
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" s="86" t="s">
         <v>217</v>
       </c>
-      <c r="B14" s="75"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="60"/>
       <c r="D14" s="60"/>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
       <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
+      <c r="H14" s="60">
+        <v>0.88</v>
+      </c>
       <c r="I14" s="60">
+        <v>0</v>
+      </c>
+      <c r="J14" s="60">
         <v>0.88</v>
       </c>
-      <c r="J14" s="60">
-        <v>0</v>
-      </c>
       <c r="K14" s="60">
-        <v>0.88</v>
-      </c>
-      <c r="L14" s="60">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L14" s="60"/>
       <c r="M14" s="60"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
@@ -15496,31 +15477,30 @@
       <c r="AA14" s="60"/>
       <c r="AB14" s="60"/>
       <c r="AC14" s="60"/>
-      <c r="AD14" s="60"/>
-    </row>
-    <row r="15" spans="1:30">
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15" s="86" t="s">
         <v>169</v>
       </c>
-      <c r="B15" s="74"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="59"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
       <c r="F15" s="59"/>
       <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
+      <c r="H15" s="59">
+        <v>0.88</v>
+      </c>
       <c r="I15" s="59">
+        <v>0</v>
+      </c>
+      <c r="J15" s="59">
         <v>0.88</v>
       </c>
-      <c r="J15" s="59">
-        <v>0</v>
-      </c>
       <c r="K15" s="59">
-        <v>0.88</v>
-      </c>
-      <c r="L15" s="59">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L15" s="59"/>
       <c r="M15" s="59"/>
       <c r="N15" s="59"/>
       <c r="O15" s="59"/>
@@ -15538,31 +15518,30 @@
       <c r="AA15" s="59"/>
       <c r="AB15" s="59"/>
       <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-    </row>
-    <row r="16" spans="1:30">
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="75"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="60"/>
       <c r="D16" s="60"/>
       <c r="E16" s="60"/>
       <c r="F16" s="60"/>
       <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
+      <c r="H16" s="60">
+        <v>0.88</v>
+      </c>
       <c r="I16" s="60">
+        <v>0</v>
+      </c>
+      <c r="J16" s="60">
         <v>0.88</v>
       </c>
-      <c r="J16" s="60">
-        <v>0</v>
-      </c>
       <c r="K16" s="60">
-        <v>0.88</v>
-      </c>
-      <c r="L16" s="60">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L16" s="60"/>
       <c r="M16" s="60"/>
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
@@ -15580,31 +15559,30 @@
       <c r="AA16" s="60"/>
       <c r="AB16" s="60"/>
       <c r="AC16" s="60"/>
-      <c r="AD16" s="60"/>
-    </row>
-    <row r="17" spans="1:30">
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="B17" s="74"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="59"/>
       <c r="D17" s="59"/>
       <c r="E17" s="59"/>
       <c r="F17" s="59"/>
       <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
+      <c r="H17" s="59">
+        <v>0.88</v>
+      </c>
       <c r="I17" s="59">
+        <v>0</v>
+      </c>
+      <c r="J17" s="59">
         <v>0.88</v>
       </c>
-      <c r="J17" s="59">
-        <v>0</v>
-      </c>
       <c r="K17" s="59">
-        <v>0.88</v>
-      </c>
-      <c r="L17" s="59">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L17" s="59"/>
       <c r="M17" s="59"/>
       <c r="N17" s="59"/>
       <c r="O17" s="59"/>
@@ -15622,31 +15600,30 @@
       <c r="AA17" s="59"/>
       <c r="AB17" s="59"/>
       <c r="AC17" s="59"/>
-      <c r="AD17" s="59"/>
-    </row>
-    <row r="18" spans="1:30">
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="B18" s="75"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="60"/>
       <c r="D18" s="60"/>
       <c r="E18" s="60"/>
       <c r="F18" s="60"/>
       <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
+      <c r="H18" s="60">
+        <v>0.88</v>
+      </c>
       <c r="I18" s="60">
+        <v>0</v>
+      </c>
+      <c r="J18" s="60">
         <v>0.88</v>
       </c>
-      <c r="J18" s="60">
-        <v>0</v>
-      </c>
       <c r="K18" s="60">
-        <v>0.88</v>
-      </c>
-      <c r="L18" s="60">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L18" s="60"/>
       <c r="M18" s="60"/>
       <c r="N18" s="60"/>
       <c r="O18" s="60"/>
@@ -15664,13 +15641,12 @@
       <c r="AA18" s="60"/>
       <c r="AB18" s="60"/>
       <c r="AC18" s="60"/>
-      <c r="AD18" s="60"/>
-    </row>
-    <row r="19" spans="1:30">
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="B19" s="74"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
@@ -15698,13 +15674,12 @@
       <c r="AA19" s="59"/>
       <c r="AB19" s="59"/>
       <c r="AC19" s="59"/>
-      <c r="AD19" s="59"/>
-    </row>
-    <row r="20" spans="1:30">
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="B20" s="75"/>
+      <c r="B20" s="60"/>
       <c r="C20" s="60"/>
       <c r="D20" s="60"/>
       <c r="E20" s="60"/>
@@ -15716,13 +15691,13 @@
       <c r="K20" s="60"/>
       <c r="L20" s="60"/>
       <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
+      <c r="N20" s="60">
+        <v>0.98</v>
+      </c>
       <c r="O20" s="60">
         <v>0.98</v>
       </c>
-      <c r="P20" s="60">
-        <v>0.98</v>
-      </c>
+      <c r="P20" s="60"/>
       <c r="Q20" s="60"/>
       <c r="R20" s="60"/>
       <c r="S20" s="60"/>
@@ -15736,13 +15711,12 @@
       <c r="AA20" s="60"/>
       <c r="AB20" s="60"/>
       <c r="AC20" s="60"/>
-      <c r="AD20" s="60"/>
-    </row>
-    <row r="21" spans="1:30">
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="B21" s="74"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
@@ -15754,13 +15728,13 @@
       <c r="K21" s="59"/>
       <c r="L21" s="59"/>
       <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
+      <c r="N21" s="59">
+        <v>0.98</v>
+      </c>
       <c r="O21" s="59">
         <v>0.98</v>
       </c>
-      <c r="P21" s="59">
-        <v>0.98</v>
-      </c>
+      <c r="P21" s="59"/>
       <c r="Q21" s="59"/>
       <c r="R21" s="59"/>
       <c r="S21" s="59"/>
@@ -15774,13 +15748,12 @@
       <c r="AA21" s="59"/>
       <c r="AB21" s="59"/>
       <c r="AC21" s="59"/>
-      <c r="AD21" s="59"/>
-    </row>
-    <row r="22" spans="1:30">
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22" s="86" t="s">
         <v>176</v>
       </c>
-      <c r="B22" s="75"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="60"/>
       <c r="D22" s="60"/>
       <c r="E22" s="60"/>
@@ -15794,13 +15767,13 @@
       <c r="M22" s="60"/>
       <c r="N22" s="60"/>
       <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
+      <c r="P22" s="60">
+        <v>0.88</v>
+      </c>
       <c r="Q22" s="60">
         <v>0.88</v>
       </c>
-      <c r="R22" s="60">
-        <v>0.88</v>
-      </c>
+      <c r="R22" s="60"/>
       <c r="S22" s="60"/>
       <c r="T22" s="60"/>
       <c r="U22" s="60"/>
@@ -15812,13 +15785,12 @@
       <c r="AA22" s="60"/>
       <c r="AB22" s="60"/>
       <c r="AC22" s="60"/>
-      <c r="AD22" s="60"/>
-    </row>
-    <row r="23" spans="1:30">
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23" s="86" t="s">
         <v>177</v>
       </c>
-      <c r="B23" s="74"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="59"/>
       <c r="D23" s="59"/>
       <c r="E23" s="59"/>
@@ -15846,13 +15818,12 @@
       <c r="AA23" s="59"/>
       <c r="AB23" s="59"/>
       <c r="AC23" s="59"/>
-      <c r="AD23" s="59"/>
-    </row>
-    <row r="24" spans="1:30">
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" s="86" t="s">
         <v>178</v>
       </c>
-      <c r="B24" s="75"/>
+      <c r="B24" s="60"/>
       <c r="C24" s="60"/>
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
@@ -15880,13 +15851,12 @@
       <c r="AA24" s="60"/>
       <c r="AB24" s="60"/>
       <c r="AC24" s="60"/>
-      <c r="AD24" s="60"/>
-    </row>
-    <row r="25" spans="1:30">
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25" s="86" t="s">
         <v>179</v>
       </c>
-      <c r="B25" s="74"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
@@ -15914,13 +15884,12 @@
       <c r="AA25" s="59"/>
       <c r="AB25" s="59"/>
       <c r="AC25" s="59"/>
-      <c r="AD25" s="59"/>
-    </row>
-    <row r="26" spans="1:30">
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26" s="86" t="s">
         <v>180</v>
       </c>
-      <c r="B26" s="75"/>
+      <c r="B26" s="60"/>
       <c r="C26" s="60"/>
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
@@ -15930,20 +15899,20 @@
       <c r="I26" s="60"/>
       <c r="J26" s="60"/>
       <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
+      <c r="L26" s="60">
+        <v>0.88</v>
+      </c>
       <c r="M26" s="60">
         <v>0.88</v>
       </c>
-      <c r="N26" s="60">
-        <v>0.88</v>
-      </c>
+      <c r="N26" s="60"/>
       <c r="O26" s="60"/>
       <c r="P26" s="60"/>
       <c r="Q26" s="60"/>
-      <c r="R26" s="60"/>
-      <c r="S26" s="60">
+      <c r="R26" s="60">
         <v>0.88</v>
       </c>
+      <c r="S26" s="60"/>
       <c r="T26" s="60"/>
       <c r="U26" s="60"/>
       <c r="V26" s="60"/>
@@ -15954,13 +15923,12 @@
       <c r="AA26" s="60"/>
       <c r="AB26" s="60"/>
       <c r="AC26" s="60"/>
-      <c r="AD26" s="60"/>
-    </row>
-    <row r="27" spans="1:30">
+    </row>
+    <row r="27" spans="1:29">
       <c r="A27" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="B27" s="74"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="59"/>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
@@ -15988,21 +15956,20 @@
       <c r="AA27" s="59"/>
       <c r="AB27" s="59"/>
       <c r="AC27" s="59"/>
-      <c r="AD27" s="59"/>
-    </row>
-    <row r="28" spans="1:30">
+    </row>
+    <row r="28" spans="1:29">
       <c r="A28" s="86" t="s">
         <v>182</v>
       </c>
-      <c r="B28" s="75"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
+      <c r="D28" s="60">
+        <v>0.88</v>
+      </c>
       <c r="E28" s="60">
         <v>0.88</v>
       </c>
-      <c r="F28" s="60">
-        <v>0.88</v>
-      </c>
+      <c r="F28" s="60"/>
       <c r="G28" s="60"/>
       <c r="H28" s="60"/>
       <c r="I28" s="60"/>
@@ -16026,21 +15993,20 @@
       <c r="AA28" s="60"/>
       <c r="AB28" s="60"/>
       <c r="AC28" s="60"/>
-      <c r="AD28" s="60"/>
-    </row>
-    <row r="29" spans="1:30">
+    </row>
+    <row r="29" spans="1:29">
       <c r="A29" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="B29" s="74"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
+      <c r="D29" s="59">
+        <v>0.88</v>
+      </c>
       <c r="E29" s="59">
         <v>0.88</v>
       </c>
-      <c r="F29" s="59">
-        <v>0.88</v>
-      </c>
+      <c r="F29" s="59"/>
       <c r="G29" s="59"/>
       <c r="H29" s="59"/>
       <c r="I29" s="59"/>
@@ -16064,19 +16030,18 @@
       <c r="AA29" s="59"/>
       <c r="AB29" s="59"/>
       <c r="AC29" s="59"/>
-      <c r="AD29" s="59"/>
-    </row>
-    <row r="30" spans="1:30">
+    </row>
+    <row r="30" spans="1:29">
       <c r="A30" s="86" t="s">
         <v>184</v>
       </c>
-      <c r="B30" s="75"/>
+      <c r="B30" s="60">
+        <v>0.88</v>
+      </c>
       <c r="C30" s="60">
         <v>0.88</v>
       </c>
-      <c r="D30" s="60">
-        <v>0.88</v>
-      </c>
+      <c r="D30" s="60"/>
       <c r="E30" s="60"/>
       <c r="F30" s="60"/>
       <c r="G30" s="60"/>
@@ -16102,19 +16067,18 @@
       <c r="AA30" s="60"/>
       <c r="AB30" s="60"/>
       <c r="AC30" s="60"/>
-      <c r="AD30" s="60"/>
-    </row>
-    <row r="31" spans="1:30">
+    </row>
+    <row r="31" spans="1:29">
       <c r="A31" s="86" t="s">
         <v>185</v>
       </c>
-      <c r="B31" s="74"/>
+      <c r="B31" s="59">
+        <v>0.88</v>
+      </c>
       <c r="C31" s="59">
         <v>0.88</v>
       </c>
-      <c r="D31" s="59">
-        <v>0.88</v>
-      </c>
+      <c r="D31" s="59"/>
       <c r="E31" s="59"/>
       <c r="F31" s="59"/>
       <c r="G31" s="59"/>
@@ -16140,19 +16104,18 @@
       <c r="AA31" s="59"/>
       <c r="AB31" s="59"/>
       <c r="AC31" s="59"/>
-      <c r="AD31" s="59"/>
-    </row>
-    <row r="32" spans="1:30">
+    </row>
+    <row r="32" spans="1:29">
       <c r="A32" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="B32" s="75"/>
+      <c r="B32" s="60">
+        <v>0.88</v>
+      </c>
       <c r="C32" s="60">
         <v>0.88</v>
       </c>
-      <c r="D32" s="60">
-        <v>0.88</v>
-      </c>
+      <c r="D32" s="60"/>
       <c r="E32" s="60"/>
       <c r="F32" s="60"/>
       <c r="G32" s="60"/>
@@ -16178,21 +16141,20 @@
       <c r="AA32" s="60"/>
       <c r="AB32" s="60"/>
       <c r="AC32" s="60"/>
-      <c r="AD32" s="60"/>
-    </row>
-    <row r="33" spans="1:30">
+    </row>
+    <row r="33" spans="1:29">
       <c r="A33" s="86" t="s">
         <v>187</v>
       </c>
-      <c r="B33" s="74"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
+      <c r="D33" s="59">
+        <v>0.88</v>
+      </c>
       <c r="E33" s="59">
         <v>0.88</v>
       </c>
-      <c r="F33" s="59">
-        <v>0.88</v>
-      </c>
+      <c r="F33" s="59"/>
       <c r="G33" s="59"/>
       <c r="H33" s="59"/>
       <c r="I33" s="59"/>
@@ -16216,19 +16178,18 @@
       <c r="AA33" s="59"/>
       <c r="AB33" s="59"/>
       <c r="AC33" s="59"/>
-      <c r="AD33" s="59"/>
-    </row>
-    <row r="34" spans="1:30">
+    </row>
+    <row r="34" spans="1:29">
       <c r="A34" s="86" t="s">
         <v>188</v>
       </c>
-      <c r="B34" s="75"/>
+      <c r="B34" s="60">
+        <v>0.88</v>
+      </c>
       <c r="C34" s="60">
         <v>0.88</v>
       </c>
-      <c r="D34" s="60">
-        <v>0.88</v>
-      </c>
+      <c r="D34" s="60"/>
       <c r="E34" s="60"/>
       <c r="F34" s="60"/>
       <c r="G34" s="60"/>
@@ -16254,13 +16215,12 @@
       <c r="AA34" s="60"/>
       <c r="AB34" s="60"/>
       <c r="AC34" s="60"/>
-      <c r="AD34" s="60"/>
-    </row>
-    <row r="35" spans="1:30">
+    </row>
+    <row r="35" spans="1:29">
       <c r="A35" s="86" t="s">
         <v>189</v>
       </c>
-      <c r="B35" s="74"/>
+      <c r="B35" s="59"/>
       <c r="C35" s="59"/>
       <c r="D35" s="59"/>
       <c r="E35" s="59"/>
@@ -16279,26 +16239,25 @@
       <c r="R35" s="59"/>
       <c r="S35" s="59"/>
       <c r="T35" s="59"/>
-      <c r="U35" s="59"/>
-      <c r="V35" s="59">
+      <c r="U35" s="59">
         <v>0.88</v>
       </c>
-      <c r="W35" s="59"/>
-      <c r="X35" s="59">
+      <c r="V35" s="59"/>
+      <c r="W35" s="59">
         <v>0.88</v>
       </c>
+      <c r="X35" s="59"/>
       <c r="Y35" s="59"/>
       <c r="Z35" s="59"/>
       <c r="AA35" s="59"/>
       <c r="AB35" s="59"/>
       <c r="AC35" s="59"/>
-      <c r="AD35" s="59"/>
-    </row>
-    <row r="36" spans="1:30">
+    </row>
+    <row r="36" spans="1:29">
       <c r="A36" s="86" t="s">
         <v>190</v>
       </c>
-      <c r="B36" s="75"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="60"/>
       <c r="D36" s="60"/>
       <c r="E36" s="60"/>
@@ -16317,26 +16276,25 @@
       <c r="R36" s="60"/>
       <c r="S36" s="60"/>
       <c r="T36" s="60"/>
-      <c r="U36" s="60"/>
-      <c r="V36" s="60">
+      <c r="U36" s="60">
         <v>0.88</v>
       </c>
-      <c r="W36" s="60"/>
-      <c r="X36" s="60">
+      <c r="V36" s="60"/>
+      <c r="W36" s="60">
         <v>0.88</v>
       </c>
+      <c r="X36" s="60"/>
       <c r="Y36" s="60"/>
       <c r="Z36" s="60"/>
       <c r="AA36" s="60"/>
       <c r="AB36" s="60"/>
       <c r="AC36" s="60"/>
-      <c r="AD36" s="60"/>
-    </row>
-    <row r="37" spans="1:30">
+    </row>
+    <row r="37" spans="1:29">
       <c r="A37" s="86" t="s">
         <v>191</v>
       </c>
-      <c r="B37" s="74"/>
+      <c r="B37" s="59"/>
       <c r="C37" s="59"/>
       <c r="D37" s="59"/>
       <c r="E37" s="59"/>
@@ -16355,26 +16313,25 @@
       <c r="R37" s="59"/>
       <c r="S37" s="59"/>
       <c r="T37" s="59"/>
-      <c r="U37" s="59"/>
-      <c r="V37" s="59">
+      <c r="U37" s="59">
         <v>0.88</v>
       </c>
-      <c r="W37" s="59"/>
-      <c r="X37" s="59">
+      <c r="V37" s="59"/>
+      <c r="W37" s="59">
         <v>0.88</v>
       </c>
+      <c r="X37" s="59"/>
       <c r="Y37" s="59"/>
       <c r="Z37" s="59"/>
       <c r="AA37" s="59"/>
       <c r="AB37" s="59"/>
       <c r="AC37" s="59"/>
-      <c r="AD37" s="59"/>
-    </row>
-    <row r="38" spans="1:30">
+    </row>
+    <row r="38" spans="1:29">
       <c r="A38" s="86" t="s">
         <v>192</v>
       </c>
-      <c r="B38" s="75"/>
+      <c r="B38" s="60"/>
       <c r="C38" s="60"/>
       <c r="D38" s="60"/>
       <c r="E38" s="60"/>
@@ -16393,10 +16350,10 @@
       <c r="R38" s="60"/>
       <c r="S38" s="60"/>
       <c r="T38" s="60"/>
-      <c r="U38" s="60"/>
-      <c r="V38" s="60">
+      <c r="U38" s="60">
         <v>0.88</v>
       </c>
+      <c r="V38" s="60"/>
       <c r="W38" s="60"/>
       <c r="X38" s="60"/>
       <c r="Y38" s="60"/>
@@ -16404,13 +16361,12 @@
       <c r="AA38" s="60"/>
       <c r="AB38" s="60"/>
       <c r="AC38" s="60"/>
-      <c r="AD38" s="60"/>
-    </row>
-    <row r="39" spans="1:30">
+    </row>
+    <row r="39" spans="1:29">
       <c r="A39" s="86" t="s">
         <v>193</v>
       </c>
-      <c r="B39" s="74"/>
+      <c r="B39" s="59"/>
       <c r="C39" s="59"/>
       <c r="D39" s="59"/>
       <c r="E39" s="59"/>
@@ -16429,10 +16385,10 @@
       <c r="R39" s="59"/>
       <c r="S39" s="59"/>
       <c r="T39" s="59"/>
-      <c r="U39" s="59"/>
-      <c r="V39" s="59">
+      <c r="U39" s="59">
         <v>0.88</v>
       </c>
+      <c r="V39" s="59"/>
       <c r="W39" s="59"/>
       <c r="X39" s="59"/>
       <c r="Y39" s="59"/>
@@ -16440,13 +16396,12 @@
       <c r="AA39" s="59"/>
       <c r="AB39" s="59"/>
       <c r="AC39" s="59"/>
-      <c r="AD39" s="59"/>
-    </row>
-    <row r="40" spans="1:30">
+    </row>
+    <row r="40" spans="1:29">
       <c r="A40" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="B40" s="75"/>
+      <c r="B40" s="60"/>
       <c r="C40" s="60"/>
       <c r="D40" s="60"/>
       <c r="E40" s="60"/>
@@ -16474,13 +16429,12 @@
       <c r="AA40" s="60"/>
       <c r="AB40" s="60"/>
       <c r="AC40" s="60"/>
-      <c r="AD40" s="60"/>
-    </row>
-    <row r="41" spans="1:30">
+    </row>
+    <row r="41" spans="1:29">
       <c r="A41" s="86" t="s">
         <v>195</v>
       </c>
-      <c r="B41" s="74"/>
+      <c r="B41" s="59"/>
       <c r="C41" s="59"/>
       <c r="D41" s="59"/>
       <c r="E41" s="59"/>
@@ -16508,13 +16462,12 @@
       <c r="AA41" s="59"/>
       <c r="AB41" s="59"/>
       <c r="AC41" s="59"/>
-      <c r="AD41" s="59"/>
-    </row>
-    <row r="42" spans="1:30">
+    </row>
+    <row r="42" spans="1:29">
       <c r="A42" s="86" t="s">
         <v>196</v>
       </c>
-      <c r="B42" s="75"/>
+      <c r="B42" s="60"/>
       <c r="C42" s="60"/>
       <c r="D42" s="60"/>
       <c r="E42" s="60"/>
@@ -16542,13 +16495,12 @@
       <c r="AA42" s="60"/>
       <c r="AB42" s="60"/>
       <c r="AC42" s="60"/>
-      <c r="AD42" s="60"/>
-    </row>
-    <row r="43" spans="1:30">
+    </row>
+    <row r="43" spans="1:29">
       <c r="A43" s="86" t="s">
         <v>197</v>
       </c>
-      <c r="B43" s="74"/>
+      <c r="B43" s="59"/>
       <c r="C43" s="59"/>
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
@@ -16576,13 +16528,12 @@
       <c r="AA43" s="59"/>
       <c r="AB43" s="59"/>
       <c r="AC43" s="59"/>
-      <c r="AD43" s="59"/>
-    </row>
-    <row r="44" spans="1:30">
+    </row>
+    <row r="44" spans="1:29">
       <c r="A44" s="86" t="s">
         <v>198</v>
       </c>
-      <c r="B44" s="75"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="60"/>
       <c r="D44" s="60"/>
       <c r="E44" s="60"/>
@@ -16610,13 +16561,12 @@
       <c r="AA44" s="60"/>
       <c r="AB44" s="60"/>
       <c r="AC44" s="60"/>
-      <c r="AD44" s="60"/>
-    </row>
-    <row r="45" spans="1:30">
+    </row>
+    <row r="45" spans="1:29">
       <c r="A45" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="B45" s="74"/>
+      <c r="B45" s="59"/>
       <c r="C45" s="59"/>
       <c r="D45" s="59"/>
       <c r="E45" s="59"/>
@@ -16644,13 +16594,12 @@
       <c r="AA45" s="59"/>
       <c r="AB45" s="59"/>
       <c r="AC45" s="59"/>
-      <c r="AD45" s="59"/>
-    </row>
-    <row r="46" spans="1:30">
+    </row>
+    <row r="46" spans="1:29">
       <c r="A46" s="86" t="s">
         <v>200</v>
       </c>
-      <c r="B46" s="75"/>
+      <c r="B46" s="60"/>
       <c r="C46" s="60"/>
       <c r="D46" s="60"/>
       <c r="E46" s="60"/>
@@ -16678,13 +16627,12 @@
       <c r="AA46" s="60"/>
       <c r="AB46" s="60"/>
       <c r="AC46" s="60"/>
-      <c r="AD46" s="60"/>
-    </row>
-    <row r="47" spans="1:30">
+    </row>
+    <row r="47" spans="1:29">
       <c r="A47" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="74"/>
+      <c r="B47" s="59"/>
       <c r="C47" s="59"/>
       <c r="D47" s="59"/>
       <c r="E47" s="59"/>
@@ -16712,13 +16660,12 @@
       <c r="AA47" s="59"/>
       <c r="AB47" s="59"/>
       <c r="AC47" s="59"/>
-      <c r="AD47" s="59"/>
-    </row>
-    <row r="48" spans="1:30">
+    </row>
+    <row r="48" spans="1:29">
       <c r="A48" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="B48" s="75"/>
+      <c r="B48" s="60"/>
       <c r="C48" s="60"/>
       <c r="D48" s="60"/>
       <c r="E48" s="60"/>
@@ -16746,13 +16693,12 @@
       <c r="AA48" s="60"/>
       <c r="AB48" s="60"/>
       <c r="AC48" s="60"/>
-      <c r="AD48" s="60"/>
-    </row>
-    <row r="49" spans="1:30">
+    </row>
+    <row r="49" spans="1:29">
       <c r="A49" s="86" t="s">
         <v>203</v>
       </c>
-      <c r="B49" s="74"/>
+      <c r="B49" s="59"/>
       <c r="C49" s="59"/>
       <c r="D49" s="59"/>
       <c r="E49" s="59"/>
@@ -16780,13 +16726,12 @@
       <c r="AA49" s="59"/>
       <c r="AB49" s="59"/>
       <c r="AC49" s="59"/>
-      <c r="AD49" s="59"/>
-    </row>
-    <row r="50" spans="1:30">
+    </row>
+    <row r="50" spans="1:29">
       <c r="A50" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="B50" s="75"/>
+      <c r="B50" s="60"/>
       <c r="C50" s="60"/>
       <c r="D50" s="60"/>
       <c r="E50" s="60"/>
@@ -16814,13 +16759,12 @@
       <c r="AA50" s="60"/>
       <c r="AB50" s="60"/>
       <c r="AC50" s="60"/>
-      <c r="AD50" s="60"/>
-    </row>
-    <row r="51" spans="1:30">
+    </row>
+    <row r="51" spans="1:29">
       <c r="A51" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="B51" s="74"/>
+      <c r="B51" s="59"/>
       <c r="C51" s="59"/>
       <c r="D51" s="59"/>
       <c r="E51" s="59"/>
@@ -16848,13 +16792,12 @@
       <c r="AA51" s="59"/>
       <c r="AB51" s="59"/>
       <c r="AC51" s="59"/>
-      <c r="AD51" s="59"/>
-    </row>
-    <row r="52" spans="1:30">
+    </row>
+    <row r="52" spans="1:29">
       <c r="A52" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="B52" s="75"/>
+      <c r="B52" s="60"/>
       <c r="C52" s="60"/>
       <c r="D52" s="60"/>
       <c r="E52" s="60"/>
@@ -16882,13 +16825,12 @@
       <c r="AA52" s="60"/>
       <c r="AB52" s="60"/>
       <c r="AC52" s="60"/>
-      <c r="AD52" s="60"/>
-    </row>
-    <row r="53" spans="1:30">
+    </row>
+    <row r="53" spans="1:29">
       <c r="A53" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="B53" s="74"/>
+      <c r="B53" s="59"/>
       <c r="C53" s="59"/>
       <c r="D53" s="59"/>
       <c r="E53" s="59"/>
@@ -16916,13 +16858,12 @@
       <c r="AA53" s="59"/>
       <c r="AB53" s="59"/>
       <c r="AC53" s="59"/>
-      <c r="AD53" s="59"/>
-    </row>
-    <row r="54" spans="1:30">
+    </row>
+    <row r="54" spans="1:29">
       <c r="A54" s="86" t="s">
         <v>208</v>
       </c>
-      <c r="B54" s="75"/>
+      <c r="B54" s="60"/>
       <c r="C54" s="60"/>
       <c r="D54" s="60"/>
       <c r="E54" s="60"/>
@@ -16950,13 +16891,12 @@
       <c r="AA54" s="60"/>
       <c r="AB54" s="60"/>
       <c r="AC54" s="60"/>
-      <c r="AD54" s="60"/>
-    </row>
-    <row r="55" spans="1:30">
+    </row>
+    <row r="55" spans="1:29">
       <c r="A55" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="B55" s="74"/>
+      <c r="B55" s="59"/>
       <c r="C55" s="59"/>
       <c r="D55" s="59"/>
       <c r="E55" s="59"/>
@@ -16984,13 +16924,12 @@
       <c r="AA55" s="59"/>
       <c r="AB55" s="59"/>
       <c r="AC55" s="59"/>
-      <c r="AD55" s="59"/>
-    </row>
-    <row r="56" spans="1:30">
+    </row>
+    <row r="56" spans="1:29">
       <c r="A56" s="86" t="s">
         <v>210</v>
       </c>
-      <c r="B56" s="75"/>
+      <c r="B56" s="60"/>
       <c r="C56" s="60"/>
       <c r="D56" s="60"/>
       <c r="E56" s="60"/>
@@ -17018,13 +16957,12 @@
       <c r="AA56" s="60"/>
       <c r="AB56" s="60"/>
       <c r="AC56" s="60"/>
-      <c r="AD56" s="60"/>
-    </row>
-    <row r="57" spans="1:30">
+    </row>
+    <row r="57" spans="1:29">
       <c r="A57" s="86" t="s">
         <v>211</v>
       </c>
-      <c r="B57" s="74"/>
+      <c r="B57" s="59"/>
       <c r="C57" s="59"/>
       <c r="D57" s="59"/>
       <c r="E57" s="59"/>
@@ -17052,13 +16990,12 @@
       <c r="AA57" s="59"/>
       <c r="AB57" s="59"/>
       <c r="AC57" s="59"/>
-      <c r="AD57" s="59"/>
-    </row>
-    <row r="58" spans="1:30">
+    </row>
+    <row r="58" spans="1:29">
       <c r="A58" s="86" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="75"/>
+      <c r="B58" s="60"/>
       <c r="C58" s="60"/>
       <c r="D58" s="60"/>
       <c r="E58" s="60"/>
@@ -17086,13 +17023,12 @@
       <c r="AA58" s="60"/>
       <c r="AB58" s="60"/>
       <c r="AC58" s="60"/>
-      <c r="AD58" s="60"/>
-    </row>
-    <row r="59" spans="1:30">
+    </row>
+    <row r="59" spans="1:29">
       <c r="A59" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="B59" s="74"/>
+      <c r="B59" s="59"/>
       <c r="C59" s="59"/>
       <c r="D59" s="59"/>
       <c r="E59" s="59"/>
@@ -17120,13 +17056,12 @@
       <c r="AA59" s="59"/>
       <c r="AB59" s="59"/>
       <c r="AC59" s="59"/>
-      <c r="AD59" s="59"/>
-    </row>
-    <row r="60" spans="1:30">
+    </row>
+    <row r="60" spans="1:29">
       <c r="A60" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="B60" s="75"/>
+      <c r="B60" s="60"/>
       <c r="C60" s="60"/>
       <c r="D60" s="60"/>
       <c r="E60" s="60"/>
@@ -17154,13 +17089,12 @@
       <c r="AA60" s="60"/>
       <c r="AB60" s="60"/>
       <c r="AC60" s="60"/>
-      <c r="AD60" s="60"/>
-    </row>
-    <row r="61" spans="1:30">
+    </row>
+    <row r="61" spans="1:29">
       <c r="A61" s="86" t="s">
         <v>215</v>
       </c>
-      <c r="B61" s="74"/>
+      <c r="B61" s="59"/>
       <c r="C61" s="59"/>
       <c r="D61" s="59"/>
       <c r="E61" s="59"/>
@@ -17188,7 +17122,6 @@
       <c r="AA61" s="59"/>
       <c r="AB61" s="59"/>
       <c r="AC61" s="59"/>
-      <c r="AD61" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17200,7 +17133,7 @@
   <dimension ref="A1:AD61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19498,8 +19431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>